<commit_message>
update machine_learning lab 8
</commit_message>
<xml_diff>
--- a/machine_learning/labs/lab_08/grid_search_results.xlsx
+++ b/machine_learning/labs/lab_08/grid_search_results.xlsx
@@ -619,16 +619,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.006861448287963867</v>
+        <v>0.01759033203125</v>
       </c>
       <c r="B2" t="n">
-        <v>0.001160451808828375</v>
+        <v>0.007672581668447013</v>
       </c>
       <c r="C2" t="n">
-        <v>0.003602123260498047</v>
+        <v>0.006675815582275391</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0003516452943996007</v>
+        <v>0.00255925973591616</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -683,16 +683,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.006808996200561523</v>
+        <v>0.01502151489257813</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0007561908659159517</v>
+        <v>0.006446823963383353</v>
       </c>
       <c r="C3" t="n">
-        <v>0.003456211090087891</v>
+        <v>0.006995105743408203</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0004872848964224761</v>
+        <v>0.003985798403965714</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -747,16 +747,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.04442963600158691</v>
+        <v>0.04792122840881348</v>
       </c>
       <c r="B4" t="n">
-        <v>0.009846603779519248</v>
+        <v>0.002505802397616665</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00746002197265625</v>
+        <v>0.007917499542236328</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0009764953097497215</v>
+        <v>0.001358262635894244</v>
       </c>
       <c r="E4" t="n">
         <v>0.1</v>
@@ -811,16 +811,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.0225306510925293</v>
+        <v>0.02304949760437012</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0032902752322402</v>
+        <v>0.0019219915185454</v>
       </c>
       <c r="C5" t="n">
-        <v>0.007429122924804688</v>
+        <v>0.007304525375366211</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001340551071414184</v>
+        <v>0.001336711819677419</v>
       </c>
       <c r="E5" t="n">
         <v>0.1</v>
@@ -875,16 +875,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.8083394050598145</v>
+        <v>0.7467369079589844</v>
       </c>
       <c r="B6" t="n">
-        <v>0.09647823862522091</v>
+        <v>0.08344985347636034</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0203371524810791</v>
+        <v>0.03389735221862793</v>
       </c>
       <c r="D6" t="n">
-        <v>0.005092937191771146</v>
+        <v>0.005117903651379063</v>
       </c>
       <c r="E6" t="n">
         <v>0.1</v>
@@ -913,7 +913,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0.986013986013986</v>
+        <v>0.993006993006993</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -928,10 +928,10 @@
         <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9972027972027971</v>
+        <v>0.9986013986013986</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.005594405594405583</v>
+        <v>0.002797202797202792</v>
       </c>
       <c r="R6" t="n">
         <v>33</v>
@@ -939,16 +939,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.1649863719940186</v>
+        <v>0.235203218460083</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0271970638769588</v>
+        <v>0.02759064963005677</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02613859176635742</v>
+        <v>0.02244892120361328</v>
       </c>
       <c r="D7" t="n">
-        <v>0.008121245592402154</v>
+        <v>0.005385141750326378</v>
       </c>
       <c r="E7" t="n">
         <v>0.1</v>
@@ -1003,16 +1003,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.02842307090759277</v>
+        <v>0.0398141860961914</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01266439742267387</v>
+        <v>0.01592453311334849</v>
       </c>
       <c r="C8" t="n">
-        <v>0.009203624725341798</v>
+        <v>0.01589388847351074</v>
       </c>
       <c r="D8" t="n">
-        <v>0.005442778923140385</v>
+        <v>0.006651422899301965</v>
       </c>
       <c r="E8" t="n">
         <v>0.1</v>
@@ -1067,16 +1067,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.02531404495239258</v>
+        <v>0.01698336601257324</v>
       </c>
       <c r="B9" t="n">
-        <v>0.01010160568141464</v>
+        <v>0.002933190126710615</v>
       </c>
       <c r="C9" t="n">
-        <v>0.009702825546264648</v>
+        <v>0.01011118888854981</v>
       </c>
       <c r="D9" t="n">
-        <v>0.003739525524370389</v>
+        <v>0.005226586712616471</v>
       </c>
       <c r="E9" t="n">
         <v>0.1</v>
@@ -1131,16 +1131,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.3872512340545654</v>
+        <v>0.4421526432037354</v>
       </c>
       <c r="B10" t="n">
-        <v>0.05441936095616666</v>
+        <v>0.04325500274647682</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01407585144042969</v>
+        <v>0.01671671867370605</v>
       </c>
       <c r="D10" t="n">
-        <v>0.004502444288076446</v>
+        <v>0.01143378264985641</v>
       </c>
       <c r="E10" t="n">
         <v>0.1</v>
@@ -1195,16 +1195,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.04747204780578614</v>
+        <v>0.03091139793395996</v>
       </c>
       <c r="B11" t="n">
-        <v>0.02526180121466264</v>
+        <v>0.009270119504159378</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0117431640625</v>
+        <v>0.010296630859375</v>
       </c>
       <c r="D11" t="n">
-        <v>0.002006918854676226</v>
+        <v>0.00334116526315895</v>
       </c>
       <c r="E11" t="n">
         <v>0.1</v>
@@ -1259,16 +1259,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>5.265609121322631</v>
+        <v>6.49530668258667</v>
       </c>
       <c r="B12" t="n">
-        <v>1.222131905736886</v>
+        <v>0.6744406879333775</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02076520919799805</v>
+        <v>0.0403740406036377</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01077636823990712</v>
+        <v>0.01591808798269742</v>
       </c>
       <c r="E12" t="n">
         <v>0.1</v>
@@ -1323,16 +1323,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.3028169631958008</v>
+        <v>0.370068883895874</v>
       </c>
       <c r="B13" t="n">
-        <v>0.08569784979452494</v>
+        <v>0.02767765583902644</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02772669792175293</v>
+        <v>0.02736468315124512</v>
       </c>
       <c r="D13" t="n">
-        <v>0.01471803577658787</v>
+        <v>0.0154946996459675</v>
       </c>
       <c r="E13" t="n">
         <v>0.1</v>
@@ -1387,16 +1387,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.0254084587097168</v>
+        <v>0.04783864021301269</v>
       </c>
       <c r="B14" t="n">
-        <v>0.00876160367845545</v>
+        <v>0.02752731973818302</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01247801780700684</v>
+        <v>0.01221551895141602</v>
       </c>
       <c r="D14" t="n">
-        <v>0.002982751062649132</v>
+        <v>0.004875522885809541</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -1451,16 +1451,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.01920328140258789</v>
+        <v>0.02346091270446777</v>
       </c>
       <c r="B15" t="n">
-        <v>0.002995200674430698</v>
+        <v>0.01425303997514766</v>
       </c>
       <c r="C15" t="n">
-        <v>0.007706928253173828</v>
+        <v>0.01011123657226562</v>
       </c>
       <c r="D15" t="n">
-        <v>0.001032113135617884</v>
+        <v>0.008353666869610385</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.07535581588745117</v>
+        <v>0.06888351440429688</v>
       </c>
       <c r="B16" t="n">
-        <v>0.02012023780227661</v>
+        <v>0.01149162879490088</v>
       </c>
       <c r="C16" t="n">
-        <v>0.009029960632324219</v>
+        <v>0.007790899276733399</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002423751429705781</v>
+        <v>0.001984415967269188</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -1579,16 +1579,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.03165740966796875</v>
+        <v>0.03221631050109863</v>
       </c>
       <c r="B17" t="n">
-        <v>0.00927026448682693</v>
+        <v>0.0171317206333989</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0132504940032959</v>
+        <v>0.009852361679077149</v>
       </c>
       <c r="D17" t="n">
-        <v>0.003779997954560949</v>
+        <v>0.002516420679548092</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -1643,16 +1643,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.9780617713928222</v>
+        <v>0.836043405532837</v>
       </c>
       <c r="B18" t="n">
-        <v>0.08929021045980844</v>
+        <v>0.126793137324449</v>
       </c>
       <c r="C18" t="n">
-        <v>0.03610396385192871</v>
+        <v>0.0248934268951416</v>
       </c>
       <c r="D18" t="n">
-        <v>0.01207493845613885</v>
+        <v>0.004251356181366276</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.1826673030853271</v>
+        <v>0.2478198051452637</v>
       </c>
       <c r="B19" t="n">
-        <v>0.03036089839761185</v>
+        <v>0.02858892560991781</v>
       </c>
       <c r="C19" t="n">
-        <v>0.02284145355224609</v>
+        <v>0.03727130889892578</v>
       </c>
       <c r="D19" t="n">
-        <v>0.001797441807514549</v>
+        <v>0.01194815200968771</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -1771,16 +1771,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.02412419319152832</v>
+        <v>0.01971545219421387</v>
       </c>
       <c r="B20" t="n">
-        <v>0.005168732884063531</v>
+        <v>0.003044496983161547</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01011366844177246</v>
+        <v>0.01030540466308594</v>
       </c>
       <c r="D20" t="n">
-        <v>0.004099878194898612</v>
+        <v>0.004702841712664912</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -1835,16 +1835,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.01550445556640625</v>
+        <v>0.02324552536010742</v>
       </c>
       <c r="B21" t="n">
-        <v>0.003871031691502264</v>
+        <v>0.00220363093248963</v>
       </c>
       <c r="C21" t="n">
-        <v>0.006992959976196289</v>
+        <v>0.01197357177734375</v>
       </c>
       <c r="D21" t="n">
-        <v>0.001736033521685897</v>
+        <v>0.003646457720912421</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -1899,16 +1899,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.4371673583984375</v>
+        <v>0.4955040454864502</v>
       </c>
       <c r="B22" t="n">
-        <v>0.07239004530689803</v>
+        <v>0.06255967315377513</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01183490753173828</v>
+        <v>0.01761660575866699</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00159456397201948</v>
+        <v>0.004939579530014752</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -1963,16 +1963,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.03421506881713867</v>
+        <v>0.04767842292785644</v>
       </c>
       <c r="B23" t="n">
-        <v>0.007649125207993857</v>
+        <v>0.007173172387494729</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01246109008789062</v>
+        <v>0.01711440086364746</v>
       </c>
       <c r="D23" t="n">
-        <v>0.003330596263203223</v>
+        <v>0.003760701253730355</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -2027,16 +2027,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>4.220325326919555</v>
+        <v>7.088434410095215</v>
       </c>
       <c r="B24" t="n">
-        <v>2.167099961642164</v>
+        <v>0.4162332285272494</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01570525169372559</v>
+        <v>0.01694059371948242</v>
       </c>
       <c r="D24" t="n">
-        <v>0.01187928908998782</v>
+        <v>0.006710194926541999</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
@@ -2091,16 +2091,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.3080463409423828</v>
+        <v>0.4547834396362305</v>
       </c>
       <c r="B25" t="n">
-        <v>0.1329096875773057</v>
+        <v>0.02482207054053146</v>
       </c>
       <c r="C25" t="n">
-        <v>0.02463216781616211</v>
+        <v>0.0587404727935791</v>
       </c>
       <c r="D25" t="n">
-        <v>0.01640031519659487</v>
+        <v>0.02203927270354503</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -2155,16 +2155,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.02551813125610352</v>
+        <v>0.03332386016845703</v>
       </c>
       <c r="B26" t="n">
-        <v>0.005221860791278515</v>
+        <v>0.008109916080554398</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01091408729553223</v>
+        <v>0.01525979042053223</v>
       </c>
       <c r="D26" t="n">
-        <v>0.002168527883951314</v>
+        <v>0.002501303641111338</v>
       </c>
       <c r="E26" t="n">
         <v>10</v>
@@ -2219,16 +2219,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.02794046401977539</v>
+        <v>0.04044013023376465</v>
       </c>
       <c r="B27" t="n">
-        <v>0.006809158918149604</v>
+        <v>0.0165255104053683</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0143439769744873</v>
+        <v>0.01703166961669922</v>
       </c>
       <c r="D27" t="n">
-        <v>0.003757719837476573</v>
+        <v>0.00789234555239466</v>
       </c>
       <c r="E27" t="n">
         <v>10</v>
@@ -2283,16 +2283,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.0841148853302002</v>
+        <v>0.0952071189880371</v>
       </c>
       <c r="B28" t="n">
-        <v>0.01625989054913772</v>
+        <v>0.01271425739540765</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01425495147705078</v>
+        <v>0.0140932559967041</v>
       </c>
       <c r="D28" t="n">
-        <v>0.003421849086832534</v>
+        <v>0.00401205762222384</v>
       </c>
       <c r="E28" t="n">
         <v>10</v>
@@ -2347,16 +2347,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.03445420265197754</v>
+        <v>0.05240187644958496</v>
       </c>
       <c r="B29" t="n">
-        <v>0.002763500231296237</v>
+        <v>0.008652041984419063</v>
       </c>
       <c r="C29" t="n">
-        <v>0.01238899230957031</v>
+        <v>0.02268242835998535</v>
       </c>
       <c r="D29" t="n">
-        <v>0.002125318778768598</v>
+        <v>0.005648735066159858</v>
       </c>
       <c r="E29" t="n">
         <v>10</v>
@@ -2411,16 +2411,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1.04179105758667</v>
+        <v>0.9355908393859863</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1679133368065987</v>
+        <v>0.1149266353038741</v>
       </c>
       <c r="C30" t="n">
-        <v>0.02476596832275391</v>
+        <v>0.03144092559814453</v>
       </c>
       <c r="D30" t="n">
-        <v>0.01026434428747391</v>
+        <v>0.008999359370066237</v>
       </c>
       <c r="E30" t="n">
         <v>10</v>
@@ -2475,16 +2475,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.2720667362213135</v>
+        <v>0.2311656475067139</v>
       </c>
       <c r="B31" t="n">
-        <v>0.05931505499501036</v>
+        <v>0.02664698545378987</v>
       </c>
       <c r="C31" t="n">
-        <v>0.03388471603393554</v>
+        <v>0.01928119659423828</v>
       </c>
       <c r="D31" t="n">
-        <v>0.01274081144148633</v>
+        <v>0.005257390503240692</v>
       </c>
       <c r="E31" t="n">
         <v>10</v>
@@ -2539,16 +2539,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.04288673400878906</v>
+        <v>0.03443975448608398</v>
       </c>
       <c r="B32" t="n">
-        <v>0.0122716642431525</v>
+        <v>0.01543106370336139</v>
       </c>
       <c r="C32" t="n">
-        <v>0.02880325317382813</v>
+        <v>0.01397705078125</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0178326475288647</v>
+        <v>0.005267408518575351</v>
       </c>
       <c r="E32" t="n">
         <v>10</v>
@@ -2603,16 +2603,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.02214512825012207</v>
+        <v>0.01841521263122559</v>
       </c>
       <c r="B33" t="n">
-        <v>0.008218333141558261</v>
+        <v>0.004136554176586337</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01078004837036133</v>
+        <v>0.006453132629394532</v>
       </c>
       <c r="D33" t="n">
-        <v>0.005884543468506124</v>
+        <v>0.0009520250197081098</v>
       </c>
       <c r="E33" t="n">
         <v>10</v>
@@ -2667,16 +2667,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.5504166126251221</v>
+        <v>0.5500071048736572</v>
       </c>
       <c r="B34" t="n">
-        <v>0.1106975157690965</v>
+        <v>0.1608256228711105</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01882243156433105</v>
+        <v>0.0249837875366211</v>
       </c>
       <c r="D34" t="n">
-        <v>0.00543825155545076</v>
+        <v>0.01240341760002157</v>
       </c>
       <c r="E34" t="n">
         <v>10</v>
@@ -2731,16 +2731,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.05009322166442871</v>
+        <v>0.04004850387573242</v>
       </c>
       <c r="B35" t="n">
-        <v>0.01605940833001256</v>
+        <v>0.001617850798150129</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01357336044311524</v>
+        <v>0.0169276237487793</v>
       </c>
       <c r="D35" t="n">
-        <v>0.002634762353718106</v>
+        <v>0.002919076124450064</v>
       </c>
       <c r="E35" t="n">
         <v>10</v>
@@ -2795,16 +2795,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>5.690765190124512</v>
+        <v>3.642265319824219</v>
       </c>
       <c r="B36" t="n">
-        <v>0.7049583909484691</v>
+        <v>0.2721318661453211</v>
       </c>
       <c r="C36" t="n">
-        <v>0.02567505836486816</v>
+        <v>0.007009077072143555</v>
       </c>
       <c r="D36" t="n">
-        <v>0.01286486965386521</v>
+        <v>0.001504746259893569</v>
       </c>
       <c r="E36" t="n">
         <v>10</v>
@@ -2859,16 +2859,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.462450647354126</v>
+        <v>0.4294622898101806</v>
       </c>
       <c r="B37" t="n">
-        <v>0.03587403140419746</v>
+        <v>0.08786427510180633</v>
       </c>
       <c r="C37" t="n">
-        <v>0.04576954841613769</v>
+        <v>0.03464741706848144</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01743388600228931</v>
+        <v>0.01871913626414119</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
@@ -3034,16 +3034,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.01586308479309082</v>
+        <v>0.01948380470275879</v>
       </c>
       <c r="B2" t="n">
-        <v>0.003635191844160187</v>
+        <v>0.002763051451326993</v>
       </c>
       <c r="C2" t="n">
-        <v>0.008152627944946289</v>
+        <v>0.008026266098022461</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001752617596248223</v>
+        <v>0.001746896658776666</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -3098,16 +3098,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01444220542907715</v>
+        <v>0.01442933082580566</v>
       </c>
       <c r="B3" t="n">
-        <v>0.0009294148020644583</v>
+        <v>0.001681344331886364</v>
       </c>
       <c r="C3" t="n">
-        <v>0.006651496887207032</v>
+        <v>0.007606029510498047</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0009948085378395977</v>
+        <v>0.00149455038623291</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -3162,16 +3162,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.3355391502380371</v>
+        <v>0.3261642932891846</v>
       </c>
       <c r="B4" t="n">
-        <v>0.01937010106785134</v>
+        <v>0.05309875384417944</v>
       </c>
       <c r="C4" t="n">
-        <v>0.08950815200805665</v>
+        <v>0.05400457382202149</v>
       </c>
       <c r="D4" t="n">
-        <v>0.01436811511207095</v>
+        <v>0.003436137941367229</v>
       </c>
       <c r="E4" t="n">
         <v>0.1</v>
@@ -3226,16 +3226,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.2216113567352295</v>
+        <v>0.235170841217041</v>
       </c>
       <c r="B5" t="n">
-        <v>0.03404426155200372</v>
+        <v>0.01659932427483089</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04411978721618652</v>
+        <v>0.02832846641540527</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0186130181234055</v>
+        <v>0.008698940305067364</v>
       </c>
       <c r="E5" t="n">
         <v>0.1</v>
@@ -3290,16 +3290,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.06216683387756348</v>
+        <v>0.05188345909118652</v>
       </c>
       <c r="B6" t="n">
-        <v>0.02426066433049061</v>
+        <v>0.02573866725091408</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01829357147216797</v>
+        <v>0.0181760311126709</v>
       </c>
       <c r="D6" t="n">
-        <v>0.008152250749363038</v>
+        <v>0.007738443147054768</v>
       </c>
       <c r="E6" t="n">
         <v>0.1</v>
@@ -3354,16 +3354,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.02476601600646973</v>
+        <v>0.01980557441711426</v>
       </c>
       <c r="B7" t="n">
-        <v>0.005699606047416776</v>
+        <v>0.006365906397238906</v>
       </c>
       <c r="C7" t="n">
-        <v>0.008472204208374023</v>
+        <v>0.009228229522705078</v>
       </c>
       <c r="D7" t="n">
-        <v>0.000810269068064442</v>
+        <v>0.005317199141449733</v>
       </c>
       <c r="E7" t="n">
         <v>0.1</v>
@@ -3418,16 +3418,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.3773630619049072</v>
+        <v>0.3913259506225586</v>
       </c>
       <c r="B8" t="n">
-        <v>0.07045319870599018</v>
+        <v>0.08107445642635074</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01598320007324219</v>
+        <v>0.02025952339172363</v>
       </c>
       <c r="D8" t="n">
-        <v>0.004566601133537383</v>
+        <v>0.01126992445953185</v>
       </c>
       <c r="E8" t="n">
         <v>0.1</v>
@@ -3482,16 +3482,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.06234583854675293</v>
+        <v>0.08178925514221191</v>
       </c>
       <c r="B9" t="n">
-        <v>0.01781816977279304</v>
+        <v>0.0459308523946324</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01451168060302734</v>
+        <v>0.01382789611816406</v>
       </c>
       <c r="D9" t="n">
-        <v>0.004680614890136789</v>
+        <v>0.005399708360042298</v>
       </c>
       <c r="E9" t="n">
         <v>0.1</v>
@@ -3546,16 +3546,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.03844919204711914</v>
+        <v>0.04508085250854492</v>
       </c>
       <c r="B10" t="n">
-        <v>0.01693457237093555</v>
+        <v>0.02214242716025515</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01299753189086914</v>
+        <v>0.01416201591491699</v>
       </c>
       <c r="D10" t="n">
-        <v>0.004352469140652503</v>
+        <v>0.003428104022788878</v>
       </c>
       <c r="E10" t="n">
         <v>0.1</v>
@@ -3610,16 +3610,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.02772531509399414</v>
+        <v>0.03564267158508301</v>
       </c>
       <c r="B11" t="n">
-        <v>0.006799139640265218</v>
+        <v>0.01011568839605383</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01443314552307129</v>
+        <v>0.01429157257080078</v>
       </c>
       <c r="D11" t="n">
-        <v>0.01071583776394548</v>
+        <v>0.00330125206206295</v>
       </c>
       <c r="E11" t="n">
         <v>0.1</v>
@@ -3674,16 +3674,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.2483139991760254</v>
+        <v>0.2577434539794922</v>
       </c>
       <c r="B12" t="n">
-        <v>0.02964074040151518</v>
+        <v>0.1174105678581004</v>
       </c>
       <c r="C12" t="n">
-        <v>0.08819055557250977</v>
+        <v>0.09125571250915528</v>
       </c>
       <c r="D12" t="n">
-        <v>0.006562059872030535</v>
+        <v>0.03702329886074172</v>
       </c>
       <c r="E12" t="n">
         <v>0.1</v>
@@ -3738,16 +3738,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.239201545715332</v>
+        <v>0.2954594135284424</v>
       </c>
       <c r="B13" t="n">
-        <v>0.05971886305027362</v>
+        <v>0.0853920904155694</v>
       </c>
       <c r="C13" t="n">
-        <v>0.11312575340271</v>
+        <v>0.0812753677368164</v>
       </c>
       <c r="D13" t="n">
-        <v>0.04564696660439726</v>
+        <v>0.0162705758403405</v>
       </c>
       <c r="E13" t="n">
         <v>0.1</v>
@@ -3802,16 +3802,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.03992323875427246</v>
+        <v>0.03082914352416992</v>
       </c>
       <c r="B14" t="n">
-        <v>0.01835696072546163</v>
+        <v>0.007482995683990156</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01585783958435059</v>
+        <v>0.0117030143737793</v>
       </c>
       <c r="D14" t="n">
-        <v>0.003439803761211099</v>
+        <v>0.003618938295026523</v>
       </c>
       <c r="E14" t="n">
         <v>0.1</v>
@@ -3866,16 +3866,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.03945026397705078</v>
+        <v>0.02884716987609863</v>
       </c>
       <c r="B15" t="n">
-        <v>0.008118440077645516</v>
+        <v>0.008155477731617827</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01661577224731445</v>
+        <v>0.01297111511230469</v>
       </c>
       <c r="D15" t="n">
-        <v>0.001825689422434113</v>
+        <v>0.005297621121244878</v>
       </c>
       <c r="E15" t="n">
         <v>0.1</v>
@@ -3930,16 +3930,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.4247849941253662</v>
+        <v>0.4642256736755371</v>
       </c>
       <c r="B16" t="n">
-        <v>0.03019207264649436</v>
+        <v>0.09037849088902351</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0180811882019043</v>
+        <v>0.02040300369262695</v>
       </c>
       <c r="D16" t="n">
-        <v>0.01100649526709671</v>
+        <v>0.002920514106881127</v>
       </c>
       <c r="E16" t="n">
         <v>0.1</v>
@@ -3994,16 +3994,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.08536930084228515</v>
+        <v>0.05175671577453613</v>
       </c>
       <c r="B17" t="n">
-        <v>0.02470497920614244</v>
+        <v>0.0139133010300651</v>
       </c>
       <c r="C17" t="n">
-        <v>0.02842330932617188</v>
+        <v>0.01253194808959961</v>
       </c>
       <c r="D17" t="n">
-        <v>0.01239680379012107</v>
+        <v>0.0031611546565935</v>
       </c>
       <c r="E17" t="n">
         <v>0.1</v>
@@ -4058,16 +4058,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.02752914428710938</v>
+        <v>0.02825832366943359</v>
       </c>
       <c r="B18" t="n">
-        <v>0.006392280042909677</v>
+        <v>0.01060775720004332</v>
       </c>
       <c r="C18" t="n">
-        <v>0.008943939208984375</v>
+        <v>0.009340858459472657</v>
       </c>
       <c r="D18" t="n">
-        <v>0.001521340300507443</v>
+        <v>0.00217770907140333</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -4122,16 +4122,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.02063779830932617</v>
+        <v>0.01626763343811035</v>
       </c>
       <c r="B19" t="n">
-        <v>0.01107818198845643</v>
+        <v>0.002108367406661176</v>
       </c>
       <c r="C19" t="n">
-        <v>0.008797979354858399</v>
+        <v>0.006441354751586914</v>
       </c>
       <c r="D19" t="n">
-        <v>0.001657347429168765</v>
+        <v>0.001083672813479565</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -4186,16 +4186,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.2913229942321777</v>
+        <v>0.2465144634246826</v>
       </c>
       <c r="B20" t="n">
-        <v>0.04979327661094276</v>
+        <v>0.0436381407575455</v>
       </c>
       <c r="C20" t="n">
-        <v>0.05270013809204101</v>
+        <v>0.04159693717956543</v>
       </c>
       <c r="D20" t="n">
-        <v>0.019867195935084</v>
+        <v>0.01287206934294038</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -4250,16 +4250,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.1017604351043701</v>
+        <v>0.06553468704223633</v>
       </c>
       <c r="B21" t="n">
-        <v>0.01384470999784685</v>
+        <v>0.01162399149259167</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01943445205688477</v>
+        <v>0.02103033065795899</v>
       </c>
       <c r="D21" t="n">
-        <v>0.006849409330463113</v>
+        <v>0.007103273634953586</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -4314,16 +4314,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.02584562301635742</v>
+        <v>0.03034467697143555</v>
       </c>
       <c r="B22" t="n">
-        <v>0.006776884164395617</v>
+        <v>0.006784815105893202</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01111717224121094</v>
+        <v>0.01210713386535645</v>
       </c>
       <c r="D22" t="n">
-        <v>0.001974422027540277</v>
+        <v>0.00354947921664047</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -4378,16 +4378,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.01821131706237793</v>
+        <v>0.03664741516113281</v>
       </c>
       <c r="B23" t="n">
-        <v>0.006435658675092528</v>
+        <v>0.01096674566808661</v>
       </c>
       <c r="C23" t="n">
-        <v>0.009517383575439454</v>
+        <v>0.01976957321166992</v>
       </c>
       <c r="D23" t="n">
-        <v>0.003610976044418989</v>
+        <v>0.009166889745663771</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -4442,16 +4442,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.4118081092834472</v>
+        <v>0.3755631923675537</v>
       </c>
       <c r="B24" t="n">
-        <v>0.07063170261783294</v>
+        <v>0.04116122881721102</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01611146926879883</v>
+        <v>0.01886749267578125</v>
       </c>
       <c r="D24" t="n">
-        <v>0.003441140508517334</v>
+        <v>0.007174900004469256</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
@@ -4506,16 +4506,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.06071853637695312</v>
+        <v>0.05871124267578125</v>
       </c>
       <c r="B25" t="n">
-        <v>0.01845908537003725</v>
+        <v>0.02240989646451766</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01083846092224121</v>
+        <v>0.01051654815673828</v>
       </c>
       <c r="D25" t="n">
-        <v>0.003300359759064619</v>
+        <v>0.005084615629209348</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -4570,16 +4570,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.02707958221435547</v>
+        <v>0.02562646865844726</v>
       </c>
       <c r="B26" t="n">
-        <v>0.01025113083801627</v>
+        <v>0.01082635339673728</v>
       </c>
       <c r="C26" t="n">
-        <v>0.009656572341918945</v>
+        <v>0.01165509223937988</v>
       </c>
       <c r="D26" t="n">
-        <v>0.002094914853698407</v>
+        <v>0.008846043617009547</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
@@ -4634,16 +4634,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.02426671981811523</v>
+        <v>0.02872762680053711</v>
       </c>
       <c r="B27" t="n">
-        <v>0.01794462863585987</v>
+        <v>0.0150380404606041</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01749224662780762</v>
+        <v>0.01350569725036621</v>
       </c>
       <c r="D27" t="n">
-        <v>0.01373682028467298</v>
+        <v>0.006210444084839764</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -4698,16 +4698,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.1851054191589356</v>
+        <v>0.1251672267913818</v>
       </c>
       <c r="B28" t="n">
-        <v>0.03082424226712092</v>
+        <v>0.01365205920216024</v>
       </c>
       <c r="C28" t="n">
-        <v>0.03250894546508789</v>
+        <v>0.03494720458984375</v>
       </c>
       <c r="D28" t="n">
-        <v>0.007472695848758249</v>
+        <v>0.008276357393497219</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
@@ -4762,16 +4762,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.1459063053131104</v>
+        <v>0.1550321102142334</v>
       </c>
       <c r="B29" t="n">
-        <v>0.01512493031952847</v>
+        <v>0.01531629119159177</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02144393920898437</v>
+        <v>0.02855286598205566</v>
       </c>
       <c r="D29" t="n">
-        <v>0.003484895707392412</v>
+        <v>0.01075558572199369</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
@@ -4826,16 +4826,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.03542113304138184</v>
+        <v>0.03088803291320801</v>
       </c>
       <c r="B30" t="n">
-        <v>0.01335078075090541</v>
+        <v>0.008292146179141455</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0115532398223877</v>
+        <v>0.01307392120361328</v>
       </c>
       <c r="D30" t="n">
-        <v>0.005107817982436136</v>
+        <v>0.004889769220080741</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -4890,16 +4890,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.02926020622253418</v>
+        <v>0.02176012992858887</v>
       </c>
       <c r="B31" t="n">
-        <v>0.01096607296672898</v>
+        <v>0.006732213367712513</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01412100791931152</v>
+        <v>0.01022210121154785</v>
       </c>
       <c r="D31" t="n">
-        <v>0.007794162828776913</v>
+        <v>0.004084413897956878</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -4954,16 +4954,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.3292461395263672</v>
+        <v>0.3336957931518555</v>
       </c>
       <c r="B32" t="n">
-        <v>0.04438651615136699</v>
+        <v>0.02932009406373651</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01262431144714355</v>
+        <v>0.01147441864013672</v>
       </c>
       <c r="D32" t="n">
-        <v>0.003561583103726683</v>
+        <v>0.001377228114917613</v>
       </c>
       <c r="E32" t="n">
         <v>1</v>
@@ -5018,16 +5018,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.04836740493774414</v>
+        <v>0.05640401840209961</v>
       </c>
       <c r="B33" t="n">
-        <v>0.0133124933453247</v>
+        <v>0.02851019083334461</v>
       </c>
       <c r="C33" t="n">
-        <v>0.009530591964721679</v>
+        <v>0.01262750625610352</v>
       </c>
       <c r="D33" t="n">
-        <v>0.003183109555768563</v>
+        <v>0.004951974445845827</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
@@ -5082,16 +5082,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.02548422813415527</v>
+        <v>0.02864608764648437</v>
       </c>
       <c r="B34" t="n">
-        <v>0.007729235914425132</v>
+        <v>0.007421080663716972</v>
       </c>
       <c r="C34" t="n">
-        <v>0.006836080551147461</v>
+        <v>0.01236863136291504</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0007413747010999985</v>
+        <v>0.005758305404593382</v>
       </c>
       <c r="E34" t="n">
         <v>10</v>
@@ -5146,16 +5146,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.01689505577087402</v>
+        <v>0.02038545608520508</v>
       </c>
       <c r="B35" t="n">
-        <v>0.004152217102730781</v>
+        <v>0.00689638836653048</v>
       </c>
       <c r="C35" t="n">
-        <v>0.007386636734008789</v>
+        <v>0.01080341339111328</v>
       </c>
       <c r="D35" t="n">
-        <v>0.001539463809305065</v>
+        <v>0.00490541433053682</v>
       </c>
       <c r="E35" t="n">
         <v>10</v>
@@ -5210,16 +5210,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.1963343620300293</v>
+        <v>0.1509881019592285</v>
       </c>
       <c r="B36" t="n">
-        <v>0.008185759167504417</v>
+        <v>0.03955607719152569</v>
       </c>
       <c r="C36" t="n">
-        <v>0.02109718322753906</v>
+        <v>0.02520136833190918</v>
       </c>
       <c r="D36" t="n">
-        <v>0.003578648649768154</v>
+        <v>0.009402694936537366</v>
       </c>
       <c r="E36" t="n">
         <v>10</v>
@@ -5274,16 +5274,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.0775071144104004</v>
+        <v>0.09589581489562989</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0201161293841631</v>
+        <v>0.0243810649037597</v>
       </c>
       <c r="C37" t="n">
-        <v>0.01605286598205567</v>
+        <v>0.0235870361328125</v>
       </c>
       <c r="D37" t="n">
-        <v>0.006067800674549692</v>
+        <v>0.01446288521821553</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
@@ -5338,16 +5338,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.03456692695617676</v>
+        <v>0.02305512428283691</v>
       </c>
       <c r="B38" t="n">
-        <v>0.01330236548272918</v>
+        <v>0.005470714916416858</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0133537769317627</v>
+        <v>0.01124477386474609</v>
       </c>
       <c r="D38" t="n">
-        <v>0.006766467876428958</v>
+        <v>0.003644183537327938</v>
       </c>
       <c r="E38" t="n">
         <v>10</v>
@@ -5402,16 +5402,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.02276530265808106</v>
+        <v>0.04356164932250976</v>
       </c>
       <c r="B39" t="n">
-        <v>0.005682933445751937</v>
+        <v>0.01705446637452877</v>
       </c>
       <c r="C39" t="n">
-        <v>0.01130599975585938</v>
+        <v>0.01612629890441895</v>
       </c>
       <c r="D39" t="n">
-        <v>0.002251149857101704</v>
+        <v>0.005058119108542377</v>
       </c>
       <c r="E39" t="n">
         <v>10</v>
@@ -5466,16 +5466,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.3164071559906006</v>
+        <v>0.2961014747619629</v>
       </c>
       <c r="B40" t="n">
-        <v>0.06511438454461679</v>
+        <v>0.08924507700627292</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01346588134765625</v>
+        <v>0.01243124008178711</v>
       </c>
       <c r="D40" t="n">
-        <v>0.007952416883377233</v>
+        <v>0.007538840056691077</v>
       </c>
       <c r="E40" t="n">
         <v>10</v>
@@ -5530,16 +5530,16 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.06072330474853516</v>
+        <v>0.05639901161193848</v>
       </c>
       <c r="B41" t="n">
-        <v>0.02121659895386709</v>
+        <v>0.01032116015981558</v>
       </c>
       <c r="C41" t="n">
-        <v>0.01227927207946777</v>
+        <v>0.01019191741943359</v>
       </c>
       <c r="D41" t="n">
-        <v>0.002546291489655745</v>
+        <v>0.002024002006129505</v>
       </c>
       <c r="E41" t="n">
         <v>10</v>
@@ -5594,16 +5594,16 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.03760619163513183</v>
+        <v>0.03722858428955078</v>
       </c>
       <c r="B42" t="n">
-        <v>0.006725986152919299</v>
+        <v>0.01207142229333602</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01702046394348145</v>
+        <v>0.01416392326354981</v>
       </c>
       <c r="D42" t="n">
-        <v>0.005100021844459669</v>
+        <v>0.004560670371647072</v>
       </c>
       <c r="E42" t="n">
         <v>10</v>
@@ -5658,16 +5658,16 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.0270449161529541</v>
+        <v>0.01628227233886719</v>
       </c>
       <c r="B43" t="n">
-        <v>0.01200178958028462</v>
+        <v>0.00196848996794597</v>
       </c>
       <c r="C43" t="n">
-        <v>0.01168484687805176</v>
+        <v>0.006641483306884766</v>
       </c>
       <c r="D43" t="n">
-        <v>0.004570854339174974</v>
+        <v>0.001628257559623108</v>
       </c>
       <c r="E43" t="n">
         <v>10</v>
@@ -5722,16 +5722,16 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.1365140914916992</v>
+        <v>0.1298904895782471</v>
       </c>
       <c r="B44" t="n">
-        <v>0.02635982289911019</v>
+        <v>0.03840370215842268</v>
       </c>
       <c r="C44" t="n">
-        <v>0.03308067321777344</v>
+        <v>0.03327035903930664</v>
       </c>
       <c r="D44" t="n">
-        <v>0.01566621206777882</v>
+        <v>0.009019083751465238</v>
       </c>
       <c r="E44" t="n">
         <v>10</v>
@@ -5786,16 +5786,16 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.05744919776916504</v>
+        <v>0.05589971542358398</v>
       </c>
       <c r="B45" t="n">
-        <v>0.01409734610906511</v>
+        <v>0.009334686913607473</v>
       </c>
       <c r="C45" t="n">
-        <v>0.01339740753173828</v>
+        <v>0.01518650054931641</v>
       </c>
       <c r="D45" t="n">
-        <v>0.003164559125782354</v>
+        <v>0.005653452093341975</v>
       </c>
       <c r="E45" t="n">
         <v>10</v>
@@ -5850,16 +5850,16 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.02492742538452148</v>
+        <v>0.0292294979095459</v>
       </c>
       <c r="B46" t="n">
-        <v>0.004249659659692994</v>
+        <v>0.005383190406778263</v>
       </c>
       <c r="C46" t="n">
-        <v>0.01029930114746094</v>
+        <v>0.009924793243408203</v>
       </c>
       <c r="D46" t="n">
-        <v>0.003150355944334555</v>
+        <v>0.002703488496260394</v>
       </c>
       <c r="E46" t="n">
         <v>10</v>
@@ -5914,16 +5914,16 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.03223276138305664</v>
+        <v>0.01713428497314453</v>
       </c>
       <c r="B47" t="n">
-        <v>0.01083316279899016</v>
+        <v>0.007970305825031889</v>
       </c>
       <c r="C47" t="n">
-        <v>0.01514320373535156</v>
+        <v>0.01068720817565918</v>
       </c>
       <c r="D47" t="n">
-        <v>0.007969646727265706</v>
+        <v>0.008974173672235413</v>
       </c>
       <c r="E47" t="n">
         <v>10</v>
@@ -5978,16 +5978,16 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.1800868511199951</v>
+        <v>0.1810742378234863</v>
       </c>
       <c r="B48" t="n">
-        <v>0.09284294102155034</v>
+        <v>0.07744617658613476</v>
       </c>
       <c r="C48" t="n">
-        <v>0.00549478530883789</v>
+        <v>0.005713844299316406</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0007690408991414939</v>
+        <v>0.0003304972962993957</v>
       </c>
       <c r="E48" t="n">
         <v>10</v>
@@ -6042,16 +6042,16 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.03869314193725586</v>
+        <v>0.04582509994506836</v>
       </c>
       <c r="B49" t="n">
-        <v>0.02809741819048932</v>
+        <v>0.023982966272589</v>
       </c>
       <c r="C49" t="n">
-        <v>0.010906982421875</v>
+        <v>0.008390140533447266</v>
       </c>
       <c r="D49" t="n">
-        <v>0.007941145083407796</v>
+        <v>0.003314234844512141</v>
       </c>
       <c r="E49" t="n">
         <v>10</v>
@@ -6217,16 +6217,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.27218918800354</v>
+        <v>0.3041504859924317</v>
       </c>
       <c r="B2" t="n">
-        <v>0.01973496036308807</v>
+        <v>0.02684356271213288</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0161592960357666</v>
+        <v>0.01824502944946289</v>
       </c>
       <c r="D2" t="n">
-        <v>0.000888471433516814</v>
+        <v>0.00311039180303603</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
@@ -6273,16 +6273,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.3456806659698486</v>
+        <v>0.3159913063049317</v>
       </c>
       <c r="B3" t="n">
-        <v>0.02180812848485347</v>
+        <v>0.008502293544980312</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01755733489990234</v>
+        <v>0.01681103706359863</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001157564236106546</v>
+        <v>0.003353779861768459</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
@@ -6329,16 +6329,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.6610127925872803</v>
+        <v>0.6013609409332276</v>
       </c>
       <c r="B4" t="n">
-        <v>0.08718988881993595</v>
+        <v>0.04151242350011761</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0235844612121582</v>
+        <v>0.02651925086975098</v>
       </c>
       <c r="D4" t="n">
-        <v>0.000985532704863622</v>
+        <v>0.002967485624780861</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
@@ -6385,16 +6385,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.7409787178039551</v>
+        <v>0.6353859424591064</v>
       </c>
       <c r="B5" t="n">
-        <v>0.07023106481699376</v>
+        <v>0.02784309444329952</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02753944396972656</v>
+        <v>0.02824854850769043</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00283189127116626</v>
+        <v>0.005235236567576628</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
@@ -6441,16 +6441,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.3356391429901123</v>
+        <v>0.2982461929321289</v>
       </c>
       <c r="B6" t="n">
-        <v>0.05950095293937251</v>
+        <v>0.02386303541933906</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01808395385742188</v>
+        <v>0.01640219688415527</v>
       </c>
       <c r="D6" t="n">
-        <v>0.006805360321312627</v>
+        <v>0.001476353878261887</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
@@ -6497,16 +6497,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.3521809101104736</v>
+        <v>0.3321562767028808</v>
       </c>
       <c r="B7" t="n">
-        <v>0.02932405021746287</v>
+        <v>0.03002600910346339</v>
       </c>
       <c r="C7" t="n">
-        <v>0.018719482421875</v>
+        <v>0.01755051612854004</v>
       </c>
       <c r="D7" t="n">
-        <v>0.002722748513384336</v>
+        <v>0.002729926589689211</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
@@ -6553,16 +6553,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.5322170257568359</v>
+        <v>0.568495512008667</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01830927836598852</v>
+        <v>0.03528830253998393</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02266926765441895</v>
+        <v>0.02538962364196777</v>
       </c>
       <c r="D8" t="n">
-        <v>0.001234013655882113</v>
+        <v>0.003408777767616983</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
@@ -6609,16 +6609,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.6599376201629639</v>
+        <v>0.6422585010528564</v>
       </c>
       <c r="B9" t="n">
-        <v>0.04496089881639979</v>
+        <v>0.08092967453851896</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02871627807617188</v>
+        <v>0.02653837203979492</v>
       </c>
       <c r="D9" t="n">
-        <v>0.004053990307327734</v>
+        <v>0.00236050104331201</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
@@ -6665,16 +6665,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2975856781005859</v>
+        <v>0.2927299499511719</v>
       </c>
       <c r="B10" t="n">
-        <v>0.03765184339767626</v>
+        <v>0.03186376028896629</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01401867866516113</v>
+        <v>0.01687984466552734</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0009201272825168355</v>
+        <v>0.002843801393455058</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
@@ -6721,16 +6721,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.3257953643798828</v>
+        <v>0.3483455657958984</v>
       </c>
       <c r="B11" t="n">
-        <v>0.011682784389085</v>
+        <v>0.04667947726046948</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01657013893127441</v>
+        <v>0.0209136962890625</v>
       </c>
       <c r="D11" t="n">
-        <v>0.002149679714633214</v>
+        <v>0.006915333607795914</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
@@ -6777,16 +6777,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.5577617168426514</v>
+        <v>0.5743406295776368</v>
       </c>
       <c r="B12" t="n">
-        <v>0.03440290716111279</v>
+        <v>0.04510222661339556</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02311816215515137</v>
+        <v>0.02414383888244629</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0006405578542736394</v>
+        <v>0.001078669455923698</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
@@ -6833,16 +6833,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.6596768379211426</v>
+        <v>0.6618286609649658</v>
       </c>
       <c r="B13" t="n">
-        <v>0.05378897373407746</v>
+        <v>0.04263695678026605</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02616767883300781</v>
+        <v>0.02734708786010742</v>
       </c>
       <c r="D13" t="n">
-        <v>0.002285309323936862</v>
+        <v>0.002998317698289188</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
@@ -6889,16 +6889,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.2851054668426514</v>
+        <v>0.2881369113922119</v>
       </c>
       <c r="B14" t="n">
-        <v>0.01110987687920225</v>
+        <v>0.03529091216723228</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01507482528686523</v>
+        <v>0.0153684139251709</v>
       </c>
       <c r="D14" t="n">
-        <v>0.001020981544586541</v>
+        <v>0.001495070114353302</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
@@ -6945,16 +6945,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.3254783153533936</v>
+        <v>0.3654116630554199</v>
       </c>
       <c r="B15" t="n">
-        <v>0.02525917664396087</v>
+        <v>0.03590513550709444</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0164924144744873</v>
+        <v>0.03606739044189453</v>
       </c>
       <c r="D15" t="n">
-        <v>0.001773810831295058</v>
+        <v>0.01281769059636913</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
@@ -7001,16 +7001,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.565199613571167</v>
+        <v>0.6560186386108399</v>
       </c>
       <c r="B16" t="n">
-        <v>0.03986929938598379</v>
+        <v>0.04081842867977352</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02578535079956055</v>
+        <v>0.02687735557556152</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002807365365208986</v>
+        <v>0.004194709628792067</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
@@ -7057,16 +7057,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.6384788990020752</v>
+        <v>0.7490833282470704</v>
       </c>
       <c r="B17" t="n">
-        <v>0.04885468412315256</v>
+        <v>0.06797479502579927</v>
       </c>
       <c r="C17" t="n">
-        <v>0.02660584449768066</v>
+        <v>0.02671570777893066</v>
       </c>
       <c r="D17" t="n">
-        <v>0.002899624301100138</v>
+        <v>0.003563874458795069</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
@@ -7113,16 +7113,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.2943907260894775</v>
+        <v>0.2876410007476807</v>
       </c>
       <c r="B18" t="n">
-        <v>0.02467287164979825</v>
+        <v>0.01587345835070982</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01559419631958008</v>
+        <v>0.01472830772399902</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00190008314124953</v>
+        <v>0.001158625232350626</v>
       </c>
       <c r="E18" t="n">
         <v>10</v>
@@ -7171,16 +7171,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.3205539226531983</v>
+        <v>0.334312105178833</v>
       </c>
       <c r="B19" t="n">
-        <v>0.01818368248440778</v>
+        <v>0.02550444749026195</v>
       </c>
       <c r="C19" t="n">
-        <v>0.01629037857055664</v>
+        <v>0.01749267578125</v>
       </c>
       <c r="D19" t="n">
-        <v>0.001057642159607864</v>
+        <v>0.001314208638246143</v>
       </c>
       <c r="E19" t="n">
         <v>10</v>
@@ -7229,16 +7229,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.5595791816711426</v>
+        <v>0.5603192329406739</v>
       </c>
       <c r="B20" t="n">
-        <v>0.02564822256787186</v>
+        <v>0.03823776563149739</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02651305198669434</v>
+        <v>0.02473893165588379</v>
       </c>
       <c r="D20" t="n">
-        <v>0.003383851586780799</v>
+        <v>0.00309266403044303</v>
       </c>
       <c r="E20" t="n">
         <v>10</v>
@@ -7287,16 +7287,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.6855872631072998</v>
+        <v>0.646356201171875</v>
       </c>
       <c r="B21" t="n">
-        <v>0.03066938242012108</v>
+        <v>0.05075980034323822</v>
       </c>
       <c r="C21" t="n">
-        <v>0.03148989677429199</v>
+        <v>0.02737584114074707</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002501824046769545</v>
+        <v>0.002990302720408264</v>
       </c>
       <c r="E21" t="n">
         <v>10</v>
@@ -7345,16 +7345,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.2694519519805908</v>
+        <v>0.2747166633605957</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0076510383096529</v>
+        <v>0.01309259421857756</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0144190788269043</v>
+        <v>0.01493315696716309</v>
       </c>
       <c r="D22" t="n">
-        <v>0.0004974399196108044</v>
+        <v>0.002599059212222494</v>
       </c>
       <c r="E22" t="n">
         <v>10</v>
@@ -7403,16 +7403,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.3199639320373535</v>
+        <v>0.3506791114807129</v>
       </c>
       <c r="B23" t="n">
-        <v>0.01586337419482809</v>
+        <v>0.03109261002636898</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0158073902130127</v>
+        <v>0.01747426986694336</v>
       </c>
       <c r="D23" t="n">
-        <v>0.001002522166539273</v>
+        <v>0.004893532875183819</v>
       </c>
       <c r="E23" t="n">
         <v>10</v>
@@ -7461,16 +7461,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.5573395729064942</v>
+        <v>0.5998172283172607</v>
       </c>
       <c r="B24" t="n">
-        <v>0.05226853832725287</v>
+        <v>0.03898136884566596</v>
       </c>
       <c r="C24" t="n">
-        <v>0.02650632858276367</v>
+        <v>0.02387576103210449</v>
       </c>
       <c r="D24" t="n">
-        <v>0.004290236559224113</v>
+        <v>0.001436262534141047</v>
       </c>
       <c r="E24" t="n">
         <v>10</v>
@@ -7519,16 +7519,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.6464538097381591</v>
+        <v>0.769077730178833</v>
       </c>
       <c r="B25" t="n">
-        <v>0.04059450488535248</v>
+        <v>0.04086404849520216</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0267977237701416</v>
+        <v>0.02660908699035645</v>
       </c>
       <c r="D25" t="n">
-        <v>0.001793080346947662</v>
+        <v>0.002691766654339782</v>
       </c>
       <c r="E25" t="n">
         <v>10</v>
@@ -7577,16 +7577,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.2781548976898193</v>
+        <v>0.3131368637084961</v>
       </c>
       <c r="B26" t="n">
-        <v>0.01056919962610014</v>
+        <v>0.05072372322914516</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01593341827392578</v>
+        <v>0.01457624435424805</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0012036817073716</v>
+        <v>0.001142133371152278</v>
       </c>
       <c r="E26" t="n">
         <v>10</v>
@@ -7635,16 +7635,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.3181487560272217</v>
+        <v>0.3604159355163574</v>
       </c>
       <c r="B27" t="n">
-        <v>0.02410753192350606</v>
+        <v>0.06534996875156514</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01619668006896973</v>
+        <v>0.01740989685058594</v>
       </c>
       <c r="D27" t="n">
-        <v>0.001681560869666729</v>
+        <v>0.003024183588432019</v>
       </c>
       <c r="E27" t="n">
         <v>10</v>
@@ -7693,16 +7693,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.5783164978027344</v>
+        <v>0.5760008335113526</v>
       </c>
       <c r="B28" t="n">
-        <v>0.03197950029759906</v>
+        <v>0.05209653379657909</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02722330093383789</v>
+        <v>0.02462220191955566</v>
       </c>
       <c r="D28" t="n">
-        <v>0.003814283987546535</v>
+        <v>0.001449213568581359</v>
       </c>
       <c r="E28" t="n">
         <v>10</v>
@@ -7751,16 +7751,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.6601856708526611</v>
+        <v>0.6472743034362793</v>
       </c>
       <c r="B29" t="n">
-        <v>0.05455284335448412</v>
+        <v>0.0388544908732209</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0263918399810791</v>
+        <v>0.02831196784973145</v>
       </c>
       <c r="D29" t="n">
-        <v>0.001902030496114897</v>
+        <v>0.003767600729002051</v>
       </c>
       <c r="E29" t="n">
         <v>10</v>
@@ -7809,16 +7809,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.2591589450836181</v>
+        <v>0.2832871913909912</v>
       </c>
       <c r="B30" t="n">
-        <v>0.007300242586289534</v>
+        <v>0.02900935601683801</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01417436599731445</v>
+        <v>0.01744508743286133</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0008371527384919713</v>
+        <v>0.006616095482735598</v>
       </c>
       <c r="E30" t="n">
         <v>10</v>
@@ -7867,16 +7867,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.3283989906311035</v>
+        <v>0.3293128490447998</v>
       </c>
       <c r="B31" t="n">
-        <v>0.01473442366388382</v>
+        <v>0.01456741079944184</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01664290428161621</v>
+        <v>0.01599359512329102</v>
       </c>
       <c r="D31" t="n">
-        <v>0.001246261934202118</v>
+        <v>0.0005481075232026161</v>
       </c>
       <c r="E31" t="n">
         <v>10</v>
@@ -7925,16 +7925,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.5804096698760987</v>
+        <v>0.578593397140503</v>
       </c>
       <c r="B32" t="n">
-        <v>0.02738245662889258</v>
+        <v>0.06937198872100918</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0255826473236084</v>
+        <v>0.02544589042663574</v>
       </c>
       <c r="D32" t="n">
-        <v>0.003408328107718955</v>
+        <v>0.003637952682827057</v>
       </c>
       <c r="E32" t="n">
         <v>10</v>
@@ -7983,16 +7983,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.6599639892578125</v>
+        <v>0.6203779220581055</v>
       </c>
       <c r="B33" t="n">
-        <v>0.06147223235064677</v>
+        <v>0.02101219125241495</v>
       </c>
       <c r="C33" t="n">
-        <v>0.02802090644836426</v>
+        <v>0.02702302932739258</v>
       </c>
       <c r="D33" t="n">
-        <v>0.004347333465073766</v>
+        <v>0.002909662712600075</v>
       </c>
       <c r="E33" t="n">
         <v>10</v>
@@ -8041,16 +8041,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.2724163055419922</v>
+        <v>0.28537278175354</v>
       </c>
       <c r="B34" t="n">
-        <v>0.009198734975688507</v>
+        <v>0.01663880335244062</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01461277008056641</v>
+        <v>0.01450858116149902</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0009934276012262349</v>
+        <v>0.0006938072675900861</v>
       </c>
       <c r="E34" t="n">
         <v>20</v>
@@ -8099,16 +8099,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.3294816970825195</v>
+        <v>0.3396347999572754</v>
       </c>
       <c r="B35" t="n">
-        <v>0.02345587058862896</v>
+        <v>0.03914665501448995</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01536779403686523</v>
+        <v>0.01800541877746582</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0005287260719452813</v>
+        <v>0.003705842313928405</v>
       </c>
       <c r="E35" t="n">
         <v>20</v>
@@ -8157,16 +8157,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.5710292816162109</v>
+        <v>0.5518327236175538</v>
       </c>
       <c r="B36" t="n">
-        <v>0.03577254185912548</v>
+        <v>0.03322488312990739</v>
       </c>
       <c r="C36" t="n">
-        <v>0.02494416236877441</v>
+        <v>0.02389273643493652</v>
       </c>
       <c r="D36" t="n">
-        <v>0.003685112806629711</v>
+        <v>0.0008290886651857893</v>
       </c>
       <c r="E36" t="n">
         <v>20</v>
@@ -8215,16 +8215,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.6680615901947021</v>
+        <v>0.6393847465515137</v>
       </c>
       <c r="B37" t="n">
-        <v>0.02913612351740358</v>
+        <v>0.0396174015603798</v>
       </c>
       <c r="C37" t="n">
-        <v>0.02829766273498535</v>
+        <v>0.02461519241333008</v>
       </c>
       <c r="D37" t="n">
-        <v>0.003662570325829155</v>
+        <v>0.0009226496836916326</v>
       </c>
       <c r="E37" t="n">
         <v>20</v>
@@ -8273,16 +8273,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.2980832576751709</v>
+        <v>0.3029354095458984</v>
       </c>
       <c r="B38" t="n">
-        <v>0.02443592955700167</v>
+        <v>0.03067955704200262</v>
       </c>
       <c r="C38" t="n">
-        <v>0.02041325569152832</v>
+        <v>0.01475424766540527</v>
       </c>
       <c r="D38" t="n">
-        <v>0.005491595794822712</v>
+        <v>0.0005763067268824456</v>
       </c>
       <c r="E38" t="n">
         <v>20</v>
@@ -8331,16 +8331,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.3278753757476807</v>
+        <v>0.3164714336395263</v>
       </c>
       <c r="B39" t="n">
-        <v>0.01834418860537554</v>
+        <v>0.01473573748398266</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0175271987915039</v>
+        <v>0.01644024848937988</v>
       </c>
       <c r="D39" t="n">
-        <v>0.002119560185830926</v>
+        <v>0.001075519012234604</v>
       </c>
       <c r="E39" t="n">
         <v>20</v>
@@ -8389,16 +8389,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.586545753479004</v>
+        <v>0.6010930061340332</v>
       </c>
       <c r="B40" t="n">
-        <v>0.03514956817632851</v>
+        <v>0.05805725567880207</v>
       </c>
       <c r="C40" t="n">
-        <v>0.02654609680175781</v>
+        <v>0.0233522891998291</v>
       </c>
       <c r="D40" t="n">
-        <v>0.002430061652880397</v>
+        <v>0.0006114547899161266</v>
       </c>
       <c r="E40" t="n">
         <v>20</v>
@@ -8447,16 +8447,16 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.6688118934631347</v>
+        <v>0.6514202117919922</v>
       </c>
       <c r="B41" t="n">
-        <v>0.03984474070118924</v>
+        <v>0.03998738326611338</v>
       </c>
       <c r="C41" t="n">
-        <v>0.02906312942504883</v>
+        <v>0.02867279052734375</v>
       </c>
       <c r="D41" t="n">
-        <v>0.002972764159057856</v>
+        <v>0.004815856378526361</v>
       </c>
       <c r="E41" t="n">
         <v>20</v>
@@ -8505,16 +8505,16 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.2900308609008789</v>
+        <v>0.2796150207519531</v>
       </c>
       <c r="B42" t="n">
-        <v>0.01492816939648221</v>
+        <v>0.01319149708828831</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01614346504211426</v>
+        <v>0.01496405601501465</v>
       </c>
       <c r="D42" t="n">
-        <v>0.003006583382879906</v>
+        <v>0.001168446207287175</v>
       </c>
       <c r="E42" t="n">
         <v>20</v>
@@ -8563,16 +8563,16 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.3190459728240967</v>
+        <v>0.3590517044067383</v>
       </c>
       <c r="B43" t="n">
-        <v>0.01122720910387547</v>
+        <v>0.03279738657375141</v>
       </c>
       <c r="C43" t="n">
-        <v>0.01656637191772461</v>
+        <v>0.01952323913574219</v>
       </c>
       <c r="D43" t="n">
-        <v>0.002554157225035361</v>
+        <v>0.005237236142374713</v>
       </c>
       <c r="E43" t="n">
         <v>20</v>
@@ -8621,16 +8621,16 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.601174783706665</v>
+        <v>0.5831630229949951</v>
       </c>
       <c r="B44" t="n">
-        <v>0.0526738411314924</v>
+        <v>0.04671928470988205</v>
       </c>
       <c r="C44" t="n">
-        <v>0.02457647323608398</v>
+        <v>0.02399682998657227</v>
       </c>
       <c r="D44" t="n">
-        <v>0.001512675511100872</v>
+        <v>0.001833549330004531</v>
       </c>
       <c r="E44" t="n">
         <v>20</v>
@@ -8679,16 +8679,16 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.6208935260772706</v>
+        <v>0.6650797367095947</v>
       </c>
       <c r="B45" t="n">
-        <v>0.02775513148002164</v>
+        <v>0.02827654758236395</v>
       </c>
       <c r="C45" t="n">
-        <v>0.02646007537841797</v>
+        <v>0.02799720764160156</v>
       </c>
       <c r="D45" t="n">
-        <v>0.003194628701889494</v>
+        <v>0.003265277327390262</v>
       </c>
       <c r="E45" t="n">
         <v>20</v>
@@ -8737,16 +8737,16 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.2774422168731689</v>
+        <v>0.3188194274902344</v>
       </c>
       <c r="B46" t="n">
-        <v>0.03168223265766268</v>
+        <v>0.03094376164102479</v>
       </c>
       <c r="C46" t="n">
-        <v>0.01478266716003418</v>
+        <v>0.01556110382080078</v>
       </c>
       <c r="D46" t="n">
-        <v>0.001369833550973081</v>
+        <v>0.001121074460300354</v>
       </c>
       <c r="E46" t="n">
         <v>20</v>
@@ -8795,16 +8795,16 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.339962911605835</v>
+        <v>0.324685001373291</v>
       </c>
       <c r="B47" t="n">
-        <v>0.0240520530267054</v>
+        <v>0.01232352939687857</v>
       </c>
       <c r="C47" t="n">
-        <v>0.01633181571960449</v>
+        <v>0.0160771369934082</v>
       </c>
       <c r="D47" t="n">
-        <v>0.001870262513987309</v>
+        <v>0.001477546277202616</v>
       </c>
       <c r="E47" t="n">
         <v>20</v>
@@ -8853,16 +8853,16 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.5137487411499023</v>
+        <v>0.5206279754638672</v>
       </c>
       <c r="B48" t="n">
-        <v>0.03250734297501468</v>
+        <v>0.01268083147659357</v>
       </c>
       <c r="C48" t="n">
-        <v>0.01984176635742187</v>
+        <v>0.0189633846282959</v>
       </c>
       <c r="D48" t="n">
-        <v>0.003320726666872904</v>
+        <v>0.003463450571725237</v>
       </c>
       <c r="E48" t="n">
         <v>20</v>
@@ -8911,16 +8911,16 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.5108921527862549</v>
+        <v>0.5105763435363769</v>
       </c>
       <c r="B49" t="n">
-        <v>0.03782945708704525</v>
+        <v>0.04139541943980554</v>
       </c>
       <c r="C49" t="n">
-        <v>0.01404509544372559</v>
+        <v>0.01301479339599609</v>
       </c>
       <c r="D49" t="n">
-        <v>0.002208257038500781</v>
+        <v>0.000993357841354518</v>
       </c>
       <c r="E49" t="n">
         <v>20</v>
@@ -9080,16 +9080,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2948955535888672</v>
+        <v>0.2401586532592773</v>
       </c>
       <c r="B2" t="n">
-        <v>0.03096794644058757</v>
+        <v>0.009087172331574678</v>
       </c>
       <c r="C2" t="n">
-        <v>0.005884170532226562</v>
+        <v>0.004668092727661133</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001992521097472328</v>
+        <v>0.0004211451480275677</v>
       </c>
       <c r="E2" t="n">
         <v>0.01</v>
@@ -9138,16 +9138,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2.03878583908081</v>
+        <v>1.898581981658936</v>
       </c>
       <c r="B3" t="n">
-        <v>0.3020541794526561</v>
+        <v>0.2060345288182105</v>
       </c>
       <c r="C3" t="n">
-        <v>0.005101346969604492</v>
+        <v>0.005904245376586914</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0004406569696772036</v>
+        <v>0.001144679230378271</v>
       </c>
       <c r="E3" t="n">
         <v>0.01</v>
@@ -9196,16 +9196,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.273594856262207</v>
+        <v>0.2567145824432373</v>
       </c>
       <c r="B4" t="n">
-        <v>0.02169189728203185</v>
+        <v>0.01802189773903016</v>
       </c>
       <c r="C4" t="n">
-        <v>0.00674285888671875</v>
+        <v>0.004496574401855469</v>
       </c>
       <c r="D4" t="n">
-        <v>0.004160375170346791</v>
+        <v>0.0008907735848484715</v>
       </c>
       <c r="E4" t="n">
         <v>0.01</v>
@@ -9254,16 +9254,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.770934534072876</v>
+        <v>1.654277658462525</v>
       </c>
       <c r="B5" t="n">
-        <v>0.07114332387956054</v>
+        <v>0.1479305672738842</v>
       </c>
       <c r="C5" t="n">
-        <v>0.00500030517578125</v>
+        <v>0.005382490158081055</v>
       </c>
       <c r="D5" t="n">
-        <v>4.687394153994368e-05</v>
+        <v>0.0007579423511410323</v>
       </c>
       <c r="E5" t="n">
         <v>0.01</v>
@@ -9312,16 +9312,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.4602866172790527</v>
+        <v>0.4479108333587646</v>
       </c>
       <c r="B6" t="n">
-        <v>0.016916245840358</v>
+        <v>0.007294543976189943</v>
       </c>
       <c r="C6" t="n">
-        <v>0.004738283157348633</v>
+        <v>0.004062366485595703</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0005103563934877696</v>
+        <v>0.0002456434106486777</v>
       </c>
       <c r="E6" t="n">
         <v>0.01</v>
@@ -9370,16 +9370,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4.140317678451538</v>
+        <v>4.243521308898925</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6717115506349653</v>
+        <v>0.6117736078663776</v>
       </c>
       <c r="C7" t="n">
-        <v>0.005257797241210937</v>
+        <v>0.005854940414428711</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0004606013805499526</v>
+        <v>0.0008317479120643862</v>
       </c>
       <c r="E7" t="n">
         <v>0.01</v>
@@ -9428,16 +9428,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.4897852420806885</v>
+        <v>0.4484874248504639</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01466058006885245</v>
+        <v>0.02038803978618396</v>
       </c>
       <c r="C8" t="n">
-        <v>0.005864572525024414</v>
+        <v>0.004520988464355469</v>
       </c>
       <c r="D8" t="n">
-        <v>0.002778364734365765</v>
+        <v>0.000559154256872762</v>
       </c>
       <c r="E8" t="n">
         <v>0.01</v>
@@ -9486,16 +9486,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3.110356378555298</v>
+        <v>2.892759990692139</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1550762467679276</v>
+        <v>0.1761674541072087</v>
       </c>
       <c r="C9" t="n">
-        <v>0.006102514266967773</v>
+        <v>0.00531930923461914</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0008295251871925254</v>
+        <v>0.0003911865331495267</v>
       </c>
       <c r="E9" t="n">
         <v>0.01</v>
@@ -9544,16 +9544,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2815080642700195</v>
+        <v>0.2709400653839111</v>
       </c>
       <c r="B10" t="n">
-        <v>0.01548852267280831</v>
+        <v>0.02391768388550839</v>
       </c>
       <c r="C10" t="n">
-        <v>0.004713201522827148</v>
+        <v>0.004219818115234375</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0005739726051177834</v>
+        <v>0.0002452424265992402</v>
       </c>
       <c r="E10" t="n">
         <v>0.01</v>
@@ -9602,16 +9602,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.312691736221313</v>
+        <v>2.094063329696655</v>
       </c>
       <c r="B11" t="n">
-        <v>0.3165414183609306</v>
+        <v>0.4567856599838101</v>
       </c>
       <c r="C11" t="n">
-        <v>0.005325746536254883</v>
+        <v>0.005532073974609375</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0004764347858287704</v>
+        <v>0.0004811052849768247</v>
       </c>
       <c r="E11" t="n">
         <v>0.01</v>
@@ -9660,16 +9660,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.2917157173156738</v>
+        <v>0.2814150333404541</v>
       </c>
       <c r="B12" t="n">
-        <v>0.0236727208558767</v>
+        <v>0.01175634344811262</v>
       </c>
       <c r="C12" t="n">
-        <v>0.007239341735839844</v>
+        <v>0.005054140090942382</v>
       </c>
       <c r="D12" t="n">
-        <v>0.003320668905553603</v>
+        <v>0.0007657662802076743</v>
       </c>
       <c r="E12" t="n">
         <v>0.01</v>
@@ -9718,16 +9718,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.894804954528809</v>
+        <v>1.806627655029297</v>
       </c>
       <c r="B13" t="n">
-        <v>0.05884868219493347</v>
+        <v>0.09183279303018771</v>
       </c>
       <c r="C13" t="n">
-        <v>0.004832696914672851</v>
+        <v>0.005228042602539062</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0002954340962736855</v>
+        <v>0.0002571757899667009</v>
       </c>
       <c r="E13" t="n">
         <v>0.01</v>
@@ -9776,16 +9776,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.5015084266662597</v>
+        <v>0.4736497402191162</v>
       </c>
       <c r="B14" t="n">
-        <v>0.05739303315798195</v>
+        <v>0.02464794017089383</v>
       </c>
       <c r="C14" t="n">
-        <v>0.00534219741821289</v>
+        <v>0.004346418380737305</v>
       </c>
       <c r="D14" t="n">
-        <v>0.001665727051288974</v>
+        <v>0.0004849299660609243</v>
       </c>
       <c r="E14" t="n">
         <v>0.01</v>
@@ -9834,16 +9834,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5.00509467124939</v>
+        <v>5.045019054412842</v>
       </c>
       <c r="B15" t="n">
-        <v>0.9285860516183073</v>
+        <v>0.7404273992688811</v>
       </c>
       <c r="C15" t="n">
-        <v>0.005649805068969727</v>
+        <v>0.006202936172485352</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0006253061303566162</v>
+        <v>0.00133909710586234</v>
       </c>
       <c r="E15" t="n">
         <v>0.01</v>
@@ -9892,16 +9892,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.453012752532959</v>
+        <v>0.4999983787536621</v>
       </c>
       <c r="B16" t="n">
-        <v>0.02375330251600698</v>
+        <v>0.05152516055296706</v>
       </c>
       <c r="C16" t="n">
-        <v>0.004706716537475586</v>
+        <v>0.00557413101196289</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001028412670705961</v>
+        <v>0.001593796003582809</v>
       </c>
       <c r="E16" t="n">
         <v>0.01</v>
@@ -9950,16 +9950,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2.810722255706787</v>
+        <v>3.21928596496582</v>
       </c>
       <c r="B17" t="n">
-        <v>0.1888177461145982</v>
+        <v>0.08875789952259636</v>
       </c>
       <c r="C17" t="n">
-        <v>0.004942417144775391</v>
+        <v>0.005117082595825195</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00016940857261667</v>
+        <v>0.0003275178713934078</v>
       </c>
       <c r="E17" t="n">
         <v>0.01</v>
@@ -10008,16 +10008,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.1989680290222168</v>
+        <v>0.2477166175842285</v>
       </c>
       <c r="B18" t="n">
-        <v>0.01164466079848423</v>
+        <v>0.03014696982804575</v>
       </c>
       <c r="C18" t="n">
-        <v>0.00362558364868164</v>
+        <v>0.005932855606079102</v>
       </c>
       <c r="D18" t="n">
-        <v>0.0001651868392908647</v>
+        <v>0.002261874581507816</v>
       </c>
       <c r="E18" t="n">
         <v>0.1</v>
@@ -10066,16 +10066,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.5863112449646</v>
+        <v>1.747190618515015</v>
       </c>
       <c r="B19" t="n">
-        <v>0.4167005732477618</v>
+        <v>0.1922428214602743</v>
       </c>
       <c r="C19" t="n">
-        <v>0.004962682723999023</v>
+        <v>0.006471824645996094</v>
       </c>
       <c r="D19" t="n">
-        <v>0.0007614504917718302</v>
+        <v>0.002133950840396957</v>
       </c>
       <c r="E19" t="n">
         <v>0.1</v>
@@ -10124,16 +10124,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.1935188293457031</v>
+        <v>0.2167123794555664</v>
       </c>
       <c r="B20" t="n">
-        <v>0.003659938207757753</v>
+        <v>0.01250422359739094</v>
       </c>
       <c r="C20" t="n">
-        <v>0.003783464431762695</v>
+        <v>0.005112552642822265</v>
       </c>
       <c r="D20" t="n">
-        <v>0.000186046986398521</v>
+        <v>0.001987452382312324</v>
       </c>
       <c r="E20" t="n">
         <v>0.1</v>
@@ -10182,16 +10182,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.24723048210144</v>
+        <v>1.238561820983887</v>
       </c>
       <c r="B21" t="n">
-        <v>0.07493353437976676</v>
+        <v>0.07387230303769379</v>
       </c>
       <c r="C21" t="n">
-        <v>0.00558314323425293</v>
+        <v>0.004969406127929688</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0004983472248986622</v>
+        <v>0.0005009295517927941</v>
       </c>
       <c r="E21" t="n">
         <v>0.1</v>
@@ -10240,16 +10240,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.409599494934082</v>
+        <v>0.3924705982208252</v>
       </c>
       <c r="B22" t="n">
-        <v>0.0246186192313804</v>
+        <v>0.03042320613480646</v>
       </c>
       <c r="C22" t="n">
-        <v>0.004247045516967774</v>
+        <v>0.004624700546264649</v>
       </c>
       <c r="D22" t="n">
-        <v>9.66522689749481e-05</v>
+        <v>0.001032468055876938</v>
       </c>
       <c r="E22" t="n">
         <v>0.1</v>
@@ -10298,16 +10298,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>3.085968255996704</v>
+        <v>2.362762308120728</v>
       </c>
       <c r="B23" t="n">
-        <v>0.25823848420374</v>
+        <v>0.2505844605466726</v>
       </c>
       <c r="C23" t="n">
-        <v>0.005355548858642578</v>
+        <v>0.005105018615722656</v>
       </c>
       <c r="D23" t="n">
-        <v>0.0004785052780843965</v>
+        <v>0.000399264155356063</v>
       </c>
       <c r="E23" t="n">
         <v>0.1</v>
@@ -10356,16 +10356,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.4327977180480957</v>
+        <v>0.3902744293212891</v>
       </c>
       <c r="B24" t="n">
-        <v>0.04959062951048521</v>
+        <v>0.01572385880190723</v>
       </c>
       <c r="C24" t="n">
-        <v>0.004705953598022461</v>
+        <v>0.004595708847045898</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0004535540196954287</v>
+        <v>0.0005758549245751034</v>
       </c>
       <c r="E24" t="n">
         <v>0.1</v>
@@ -10414,16 +10414,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2.366840648651123</v>
+        <v>2.169717359542847</v>
       </c>
       <c r="B25" t="n">
-        <v>0.2011914482618783</v>
+        <v>0.08337673752030446</v>
       </c>
       <c r="C25" t="n">
-        <v>0.005088281631469726</v>
+        <v>0.005681180953979492</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0001962344173581947</v>
+        <v>0.001183116895259458</v>
       </c>
       <c r="E25" t="n">
         <v>0.1</v>
@@ -10472,16 +10472,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.2291605949401855</v>
+        <v>0.2140758037567139</v>
       </c>
       <c r="B26" t="n">
-        <v>0.01240623157627871</v>
+        <v>0.009819848793288099</v>
       </c>
       <c r="C26" t="n">
-        <v>0.004381799697875976</v>
+        <v>0.004513788223266602</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0004731814103942878</v>
+        <v>0.0007001414851403017</v>
       </c>
       <c r="E26" t="n">
         <v>0.1</v>
@@ -10530,16 +10530,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1.686868190765381</v>
+        <v>1.821027135848999</v>
       </c>
       <c r="B27" t="n">
-        <v>0.3165235393507051</v>
+        <v>0.3813412305592101</v>
       </c>
       <c r="C27" t="n">
-        <v>0.005545663833618164</v>
+        <v>0.004994726181030274</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0007152630233393548</v>
+        <v>0.0002251075247721263</v>
       </c>
       <c r="E27" t="n">
         <v>0.1</v>
@@ -10588,16 +10588,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.2208036899566651</v>
+        <v>0.2089676856994629</v>
       </c>
       <c r="B28" t="n">
-        <v>0.01906904875119493</v>
+        <v>0.007993444235284936</v>
       </c>
       <c r="C28" t="n">
-        <v>0.005340051651000976</v>
+        <v>0.00424036979675293</v>
       </c>
       <c r="D28" t="n">
-        <v>0.001020466438480294</v>
+        <v>0.00062359866966993</v>
       </c>
       <c r="E28" t="n">
         <v>0.1</v>
@@ -10646,16 +10646,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1.278072214126587</v>
+        <v>1.250311136245728</v>
       </c>
       <c r="B29" t="n">
-        <v>0.05751924129886481</v>
+        <v>0.05486910667510827</v>
       </c>
       <c r="C29" t="n">
-        <v>0.004789972305297851</v>
+        <v>0.004732418060302735</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0003732008476225396</v>
+        <v>0.0003103897999037927</v>
       </c>
       <c r="E29" t="n">
         <v>0.1</v>
@@ -10704,16 +10704,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.4504657745361328</v>
+        <v>0.4078182220458985</v>
       </c>
       <c r="B30" t="n">
-        <v>0.01877427552151878</v>
+        <v>0.02651471252917241</v>
       </c>
       <c r="C30" t="n">
-        <v>0.004708337783813477</v>
+        <v>0.004967164993286133</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0003896508150775843</v>
+        <v>0.001214255401810783</v>
       </c>
       <c r="E30" t="n">
         <v>0.1</v>
@@ -10762,16 +10762,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2.597908878326416</v>
+        <v>2.328103542327881</v>
       </c>
       <c r="B31" t="n">
-        <v>0.3630076506110756</v>
+        <v>0.2183064480313682</v>
       </c>
       <c r="C31" t="n">
-        <v>0.00427241325378418</v>
+        <v>0.003396463394165039</v>
       </c>
       <c r="D31" t="n">
-        <v>0.001143617290460607</v>
+        <v>0.0007654456668196479</v>
       </c>
       <c r="E31" t="n">
         <v>0.1</v>
@@ -10820,16 +10820,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.4374557971954346</v>
+        <v>0.4025423049926758</v>
       </c>
       <c r="B32" t="n">
-        <v>0.05554807333484187</v>
+        <v>0.01726131812502799</v>
       </c>
       <c r="C32" t="n">
-        <v>0.004363012313842773</v>
+        <v>0.004160118103027344</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0003086055091145505</v>
+        <v>0.0004039746393410334</v>
       </c>
       <c r="E32" t="n">
         <v>0.1</v>
@@ -10878,16 +10878,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1.882624101638794</v>
+        <v>1.756406402587891</v>
       </c>
       <c r="B33" t="n">
-        <v>0.03533795767467596</v>
+        <v>0.08980579306050827</v>
       </c>
       <c r="C33" t="n">
-        <v>0.003428840637207031</v>
+        <v>0.003134632110595703</v>
       </c>
       <c r="D33" t="n">
-        <v>0.000359183285937381</v>
+        <v>0.0002346404461938297</v>
       </c>
       <c r="E33" t="n">
         <v>0.1</v>

</xml_diff>

<commit_message>
add po_ni lab 7
</commit_message>
<xml_diff>
--- a/machine_learning/labs/lab_08/grid_search_results.xlsx
+++ b/machine_learning/labs/lab_08/grid_search_results.xlsx
@@ -619,16 +619,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.01759033203125</v>
+        <v>0.01198005676269531</v>
       </c>
       <c r="B2" t="n">
-        <v>0.007672581668447013</v>
+        <v>0.0009476076882357335</v>
       </c>
       <c r="C2" t="n">
-        <v>0.006675815582275391</v>
+        <v>0.004894542694091797</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00255925973591616</v>
+        <v>0.0003469029291989376</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -683,16 +683,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01502151489257813</v>
+        <v>0.01589970588684082</v>
       </c>
       <c r="B3" t="n">
-        <v>0.006446823963383353</v>
+        <v>0.007050606857149434</v>
       </c>
       <c r="C3" t="n">
-        <v>0.006995105743408203</v>
+        <v>0.006173324584960937</v>
       </c>
       <c r="D3" t="n">
-        <v>0.003985798403965714</v>
+        <v>0.00275656284232954</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -747,16 +747,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.04792122840881348</v>
+        <v>0.06222381591796875</v>
       </c>
       <c r="B4" t="n">
-        <v>0.002505802397616665</v>
+        <v>0.02148178264670067</v>
       </c>
       <c r="C4" t="n">
-        <v>0.007917499542236328</v>
+        <v>0.007443523406982422</v>
       </c>
       <c r="D4" t="n">
-        <v>0.001358262635894244</v>
+        <v>0.002508987150990662</v>
       </c>
       <c r="E4" t="n">
         <v>0.1</v>
@@ -811,16 +811,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.02304949760437012</v>
+        <v>0.01755175590515137</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0019219915185454</v>
+        <v>0.002326478499742708</v>
       </c>
       <c r="C5" t="n">
-        <v>0.007304525375366211</v>
+        <v>0.00552663803100586</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001336711819677419</v>
+        <v>0.001086554997189041</v>
       </c>
       <c r="E5" t="n">
         <v>0.1</v>
@@ -875,16 +875,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.7467369079589844</v>
+        <v>0.603055763244629</v>
       </c>
       <c r="B6" t="n">
-        <v>0.08344985347636034</v>
+        <v>0.04636780106161526</v>
       </c>
       <c r="C6" t="n">
-        <v>0.03389735221862793</v>
+        <v>0.0319880485534668</v>
       </c>
       <c r="D6" t="n">
-        <v>0.005117903651379063</v>
+        <v>0.01274101299471022</v>
       </c>
       <c r="E6" t="n">
         <v>0.1</v>
@@ -913,7 +913,7 @@
         </is>
       </c>
       <c r="K6" t="n">
-        <v>0.993006993006993</v>
+        <v>0.986013986013986</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -928,10 +928,10 @@
         <v>1</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9986013986013986</v>
+        <v>0.9972027972027971</v>
       </c>
       <c r="Q6" t="n">
-        <v>0.002797202797202792</v>
+        <v>0.005594405594405583</v>
       </c>
       <c r="R6" t="n">
         <v>33</v>
@@ -939,16 +939,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.235203218460083</v>
+        <v>0.1906403064727783</v>
       </c>
       <c r="B7" t="n">
-        <v>0.02759064963005677</v>
+        <v>0.04345859808136513</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02244892120361328</v>
+        <v>0.02225117683410644</v>
       </c>
       <c r="D7" t="n">
-        <v>0.005385141750326378</v>
+        <v>0.006563725541178581</v>
       </c>
       <c r="E7" t="n">
         <v>0.1</v>
@@ -1003,16 +1003,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.0398141860961914</v>
+        <v>0.01674656867980957</v>
       </c>
       <c r="B8" t="n">
-        <v>0.01592453311334849</v>
+        <v>0.002532514300076723</v>
       </c>
       <c r="C8" t="n">
-        <v>0.01589388847351074</v>
+        <v>0.006944799423217773</v>
       </c>
       <c r="D8" t="n">
-        <v>0.006651422899301965</v>
+        <v>0.0007245349520629466</v>
       </c>
       <c r="E8" t="n">
         <v>0.1</v>
@@ -1067,16 +1067,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.01698336601257324</v>
+        <v>0.02041740417480469</v>
       </c>
       <c r="B9" t="n">
-        <v>0.002933190126710615</v>
+        <v>0.005919201326686531</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01011118888854981</v>
+        <v>0.00737757682800293</v>
       </c>
       <c r="D9" t="n">
-        <v>0.005226586712616471</v>
+        <v>0.002886587552285542</v>
       </c>
       <c r="E9" t="n">
         <v>0.1</v>
@@ -1131,16 +1131,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.4421526432037354</v>
+        <v>0.3962140560150146</v>
       </c>
       <c r="B10" t="n">
-        <v>0.04325500274647682</v>
+        <v>0.0424872487102903</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01671671867370605</v>
+        <v>0.01877436637878418</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01143378264985641</v>
+        <v>0.006649839260643139</v>
       </c>
       <c r="E10" t="n">
         <v>0.1</v>
@@ -1195,16 +1195,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.03091139793395996</v>
+        <v>0.03934059143066406</v>
       </c>
       <c r="B11" t="n">
-        <v>0.009270119504159378</v>
+        <v>0.01308846673307559</v>
       </c>
       <c r="C11" t="n">
-        <v>0.010296630859375</v>
+        <v>0.01379199028015137</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00334116526315895</v>
+        <v>0.005348570660878327</v>
       </c>
       <c r="E11" t="n">
         <v>0.1</v>
@@ -1259,16 +1259,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>6.49530668258667</v>
+        <v>6.417144775390625</v>
       </c>
       <c r="B12" t="n">
-        <v>0.6744406879333775</v>
+        <v>0.260495822479391</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0403740406036377</v>
+        <v>0.04306483268737793</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01591808798269742</v>
+        <v>0.02973682495215769</v>
       </c>
       <c r="E12" t="n">
         <v>0.1</v>
@@ -1323,16 +1323,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.370068883895874</v>
+        <v>0.3091858863830567</v>
       </c>
       <c r="B13" t="n">
-        <v>0.02767765583902644</v>
+        <v>0.04736260486245322</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02736468315124512</v>
+        <v>0.03041338920593262</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0154946996459675</v>
+        <v>0.01076550497104619</v>
       </c>
       <c r="E13" t="n">
         <v>0.1</v>
@@ -1387,16 +1387,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.04783864021301269</v>
+        <v>0.02804765701293945</v>
       </c>
       <c r="B14" t="n">
-        <v>0.02752731973818302</v>
+        <v>0.01231763657177221</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01221551895141602</v>
+        <v>0.02039761543273926</v>
       </c>
       <c r="D14" t="n">
-        <v>0.004875522885809541</v>
+        <v>0.01609068161035661</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
@@ -1451,16 +1451,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.02346091270446777</v>
+        <v>0.02358417510986328</v>
       </c>
       <c r="B15" t="n">
-        <v>0.01425303997514766</v>
+        <v>0.004348869341569565</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01011123657226562</v>
+        <v>0.014306640625</v>
       </c>
       <c r="D15" t="n">
-        <v>0.008353666869610385</v>
+        <v>0.009405794296160178</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
@@ -1515,16 +1515,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.06888351440429688</v>
+        <v>0.1059271335601807</v>
       </c>
       <c r="B16" t="n">
-        <v>0.01149162879490088</v>
+        <v>0.05880806617192712</v>
       </c>
       <c r="C16" t="n">
-        <v>0.007790899276733399</v>
+        <v>0.01628456115722656</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001984415967269188</v>
+        <v>0.0107483830709407</v>
       </c>
       <c r="E16" t="n">
         <v>1</v>
@@ -1579,16 +1579,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.03221631050109863</v>
+        <v>0.04224720001220703</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0171317206333989</v>
+        <v>0.02246430681012304</v>
       </c>
       <c r="C17" t="n">
-        <v>0.009852361679077149</v>
+        <v>0.01312141418457031</v>
       </c>
       <c r="D17" t="n">
-        <v>0.002516420679548092</v>
+        <v>0.009637445763242698</v>
       </c>
       <c r="E17" t="n">
         <v>1</v>
@@ -1643,16 +1643,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.836043405532837</v>
+        <v>0.8262686729431152</v>
       </c>
       <c r="B18" t="n">
-        <v>0.126793137324449</v>
+        <v>0.1296042774983967</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0248934268951416</v>
+        <v>0.02433714866638183</v>
       </c>
       <c r="D18" t="n">
-        <v>0.004251356181366276</v>
+        <v>0.004873970724501285</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -1707,16 +1707,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.2478198051452637</v>
+        <v>0.3216852188110352</v>
       </c>
       <c r="B19" t="n">
-        <v>0.02858892560991781</v>
+        <v>0.1113461608176588</v>
       </c>
       <c r="C19" t="n">
-        <v>0.03727130889892578</v>
+        <v>0.02464933395385742</v>
       </c>
       <c r="D19" t="n">
-        <v>0.01194815200968771</v>
+        <v>0.004839191198304826</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -1771,16 +1771,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.01971545219421387</v>
+        <v>0.0217318058013916</v>
       </c>
       <c r="B20" t="n">
-        <v>0.003044496983161547</v>
+        <v>0.006986932503358526</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01030540466308594</v>
+        <v>0.006912326812744141</v>
       </c>
       <c r="D20" t="n">
-        <v>0.004702841712664912</v>
+        <v>0.0006905701948782202</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -1835,16 +1835,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.02324552536010742</v>
+        <v>0.01802339553833008</v>
       </c>
       <c r="B21" t="n">
-        <v>0.00220363093248963</v>
+        <v>0.005271083811907953</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01197357177734375</v>
+        <v>0.008058547973632812</v>
       </c>
       <c r="D21" t="n">
-        <v>0.003646457720912421</v>
+        <v>0.002776461623112851</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -1899,16 +1899,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.4955040454864502</v>
+        <v>0.5104670047760009</v>
       </c>
       <c r="B22" t="n">
-        <v>0.06255967315377513</v>
+        <v>0.1209791650635805</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01761660575866699</v>
+        <v>0.01575555801391602</v>
       </c>
       <c r="D22" t="n">
-        <v>0.004939579530014752</v>
+        <v>0.003292011145396907</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -1963,16 +1963,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.04767842292785644</v>
+        <v>0.0571476936340332</v>
       </c>
       <c r="B23" t="n">
-        <v>0.007173172387494729</v>
+        <v>0.01516431530787107</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01711440086364746</v>
+        <v>0.01894044876098633</v>
       </c>
       <c r="D23" t="n">
-        <v>0.003760701253730355</v>
+        <v>0.003482258297634069</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -2027,16 +2027,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>7.088434410095215</v>
+        <v>7.050355768203735</v>
       </c>
       <c r="B24" t="n">
-        <v>0.4162332285272494</v>
+        <v>0.4901562496455248</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01694059371948242</v>
+        <v>0.02948489189147949</v>
       </c>
       <c r="D24" t="n">
-        <v>0.006710194926541999</v>
+        <v>0.008146388174779345</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
@@ -2091,16 +2091,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.4547834396362305</v>
+        <v>0.4570487976074219</v>
       </c>
       <c r="B25" t="n">
-        <v>0.02482207054053146</v>
+        <v>0.0572147296943171</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0587404727935791</v>
+        <v>0.03857517242431641</v>
       </c>
       <c r="D25" t="n">
-        <v>0.02203927270354503</v>
+        <v>0.01079487182869684</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -2155,16 +2155,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.03332386016845703</v>
+        <v>0.04375176429748535</v>
       </c>
       <c r="B26" t="n">
-        <v>0.008109916080554398</v>
+        <v>0.003960664709951487</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01525979042053223</v>
+        <v>0.02505278587341309</v>
       </c>
       <c r="D26" t="n">
-        <v>0.002501303641111338</v>
+        <v>0.006653994626946164</v>
       </c>
       <c r="E26" t="n">
         <v>10</v>
@@ -2219,16 +2219,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.04044013023376465</v>
+        <v>0.04035072326660157</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0165255104053683</v>
+        <v>0.006600231081958519</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01703166961669922</v>
+        <v>0.02046422958374023</v>
       </c>
       <c r="D27" t="n">
-        <v>0.00789234555239466</v>
+        <v>0.006309076525935117</v>
       </c>
       <c r="E27" t="n">
         <v>10</v>
@@ -2283,16 +2283,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.0952071189880371</v>
+        <v>0.1539031505584717</v>
       </c>
       <c r="B28" t="n">
-        <v>0.01271425739540765</v>
+        <v>0.04792957652284923</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0140932559967041</v>
+        <v>0.02769045829772949</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00401205762222384</v>
+        <v>0.004209041604642435</v>
       </c>
       <c r="E28" t="n">
         <v>10</v>
@@ -2347,16 +2347,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.05240187644958496</v>
+        <v>0.07928466796875</v>
       </c>
       <c r="B29" t="n">
-        <v>0.008652041984419063</v>
+        <v>0.02318683544375668</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02268242835998535</v>
+        <v>0.0384831428527832</v>
       </c>
       <c r="D29" t="n">
-        <v>0.005648735066159858</v>
+        <v>0.02244339685692095</v>
       </c>
       <c r="E29" t="n">
         <v>10</v>
@@ -2411,16 +2411,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.9355908393859863</v>
+        <v>1.019865369796753</v>
       </c>
       <c r="B30" t="n">
-        <v>0.1149266353038741</v>
+        <v>0.1486433138093457</v>
       </c>
       <c r="C30" t="n">
-        <v>0.03144092559814453</v>
+        <v>0.03101472854614258</v>
       </c>
       <c r="D30" t="n">
-        <v>0.008999359370066237</v>
+        <v>0.01288802482890908</v>
       </c>
       <c r="E30" t="n">
         <v>10</v>
@@ -2475,16 +2475,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.2311656475067139</v>
+        <v>0.2660086631774902</v>
       </c>
       <c r="B31" t="n">
-        <v>0.02664698545378987</v>
+        <v>0.05640783162466472</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01928119659423828</v>
+        <v>0.02637968063354492</v>
       </c>
       <c r="D31" t="n">
-        <v>0.005257390503240692</v>
+        <v>0.004817564096733159</v>
       </c>
       <c r="E31" t="n">
         <v>10</v>
@@ -2539,16 +2539,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.03443975448608398</v>
+        <v>0.02374424934387207</v>
       </c>
       <c r="B32" t="n">
-        <v>0.01543106370336139</v>
+        <v>0.004389142852055546</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01397705078125</v>
+        <v>0.01077866554260254</v>
       </c>
       <c r="D32" t="n">
-        <v>0.005267408518575351</v>
+        <v>0.002776317364272295</v>
       </c>
       <c r="E32" t="n">
         <v>10</v>
@@ -2603,16 +2603,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.01841521263122559</v>
+        <v>0.02456703186035156</v>
       </c>
       <c r="B33" t="n">
-        <v>0.004136554176586337</v>
+        <v>0.004796267086974686</v>
       </c>
       <c r="C33" t="n">
-        <v>0.006453132629394532</v>
+        <v>0.01012187004089355</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0009520250197081098</v>
+        <v>0.003736785130949449</v>
       </c>
       <c r="E33" t="n">
         <v>10</v>
@@ -2667,16 +2667,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.5500071048736572</v>
+        <v>0.7025235652923584</v>
       </c>
       <c r="B34" t="n">
-        <v>0.1608256228711105</v>
+        <v>0.2190981576704042</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0249837875366211</v>
+        <v>0.03203878402709961</v>
       </c>
       <c r="D34" t="n">
-        <v>0.01240341760002157</v>
+        <v>0.0185703701161049</v>
       </c>
       <c r="E34" t="n">
         <v>10</v>
@@ -2731,16 +2731,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.04004850387573242</v>
+        <v>0.04012656211853027</v>
       </c>
       <c r="B35" t="n">
-        <v>0.001617850798150129</v>
+        <v>0.008049340036589274</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0169276237487793</v>
+        <v>0.01537704467773438</v>
       </c>
       <c r="D35" t="n">
-        <v>0.002919076124450064</v>
+        <v>0.002042248948291809</v>
       </c>
       <c r="E35" t="n">
         <v>10</v>
@@ -2795,16 +2795,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>3.642265319824219</v>
+        <v>3.596441650390625</v>
       </c>
       <c r="B36" t="n">
-        <v>0.2721318661453211</v>
+        <v>0.233927001087489</v>
       </c>
       <c r="C36" t="n">
-        <v>0.007009077072143555</v>
+        <v>0.006464672088623047</v>
       </c>
       <c r="D36" t="n">
-        <v>0.001504746259893569</v>
+        <v>0.0004472028772502385</v>
       </c>
       <c r="E36" t="n">
         <v>10</v>
@@ -2859,16 +2859,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.4294622898101806</v>
+        <v>0.4528108119964599</v>
       </c>
       <c r="B37" t="n">
-        <v>0.08786427510180633</v>
+        <v>0.04611442329754659</v>
       </c>
       <c r="C37" t="n">
-        <v>0.03464741706848144</v>
+        <v>0.03293948173522949</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01871913626414119</v>
+        <v>0.0111540168058021</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
@@ -3034,16 +3034,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.01948380470275879</v>
+        <v>0.01922941207885742</v>
       </c>
       <c r="B2" t="n">
-        <v>0.002763051451326993</v>
+        <v>0.002097400792628028</v>
       </c>
       <c r="C2" t="n">
-        <v>0.008026266098022461</v>
+        <v>0.007384109497070313</v>
       </c>
       <c r="D2" t="n">
-        <v>0.001746896658776666</v>
+        <v>0.0005224243529979882</v>
       </c>
       <c r="E2" t="n">
         <v>0.1</v>
@@ -3098,16 +3098,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.01442933082580566</v>
+        <v>0.01392664909362793</v>
       </c>
       <c r="B3" t="n">
-        <v>0.001681344331886364</v>
+        <v>0.001184735439706876</v>
       </c>
       <c r="C3" t="n">
-        <v>0.007606029510498047</v>
+        <v>0.006607770919799805</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00149455038623291</v>
+        <v>0.001800234748266558</v>
       </c>
       <c r="E3" t="n">
         <v>0.1</v>
@@ -3162,16 +3162,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.3261642932891846</v>
+        <v>0.3003021240234375</v>
       </c>
       <c r="B4" t="n">
-        <v>0.05309875384417944</v>
+        <v>0.04476070198286854</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05400457382202149</v>
+        <v>0.06249508857727051</v>
       </c>
       <c r="D4" t="n">
-        <v>0.003436137941367229</v>
+        <v>0.01677825168993279</v>
       </c>
       <c r="E4" t="n">
         <v>0.1</v>
@@ -3226,16 +3226,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.235170841217041</v>
+        <v>0.2384111404418945</v>
       </c>
       <c r="B5" t="n">
-        <v>0.01659932427483089</v>
+        <v>0.02505832331392248</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02832846641540527</v>
+        <v>0.02831349372863769</v>
       </c>
       <c r="D5" t="n">
-        <v>0.008698940305067364</v>
+        <v>0.005916674248421636</v>
       </c>
       <c r="E5" t="n">
         <v>0.1</v>
@@ -3290,16 +3290,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.05188345909118652</v>
+        <v>0.05372638702392578</v>
       </c>
       <c r="B6" t="n">
-        <v>0.02573866725091408</v>
+        <v>0.02101684451128739</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0181760311126709</v>
+        <v>0.02503757476806641</v>
       </c>
       <c r="D6" t="n">
-        <v>0.007738443147054768</v>
+        <v>0.01772364970897991</v>
       </c>
       <c r="E6" t="n">
         <v>0.1</v>
@@ -3354,16 +3354,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.01980557441711426</v>
+        <v>0.01538543701171875</v>
       </c>
       <c r="B7" t="n">
-        <v>0.006365906397238906</v>
+        <v>0.004993888955440164</v>
       </c>
       <c r="C7" t="n">
-        <v>0.009228229522705078</v>
+        <v>0.007589149475097656</v>
       </c>
       <c r="D7" t="n">
-        <v>0.005317199141449733</v>
+        <v>0.00405629465715763</v>
       </c>
       <c r="E7" t="n">
         <v>0.1</v>
@@ -3418,16 +3418,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.3913259506225586</v>
+        <v>0.3563826084136963</v>
       </c>
       <c r="B8" t="n">
-        <v>0.08107445642635074</v>
+        <v>0.06669069741755117</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02025952339172363</v>
+        <v>0.01767740249633789</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01126992445953185</v>
+        <v>0.00458880559184378</v>
       </c>
       <c r="E8" t="n">
         <v>0.1</v>
@@ -3482,16 +3482,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.08178925514221191</v>
+        <v>0.05273466110229492</v>
       </c>
       <c r="B9" t="n">
-        <v>0.0459308523946324</v>
+        <v>0.02065065775876807</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01382789611816406</v>
+        <v>0.01120338439941406</v>
       </c>
       <c r="D9" t="n">
-        <v>0.005399708360042298</v>
+        <v>0.006573048851378848</v>
       </c>
       <c r="E9" t="n">
         <v>0.1</v>
@@ -3546,16 +3546,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.04508085250854492</v>
+        <v>0.03743762969970703</v>
       </c>
       <c r="B10" t="n">
-        <v>0.02214242716025515</v>
+        <v>0.003071318253860426</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01416201591491699</v>
+        <v>0.01207156181335449</v>
       </c>
       <c r="D10" t="n">
-        <v>0.003428104022788878</v>
+        <v>0.002451635006979271</v>
       </c>
       <c r="E10" t="n">
         <v>0.1</v>
@@ -3610,16 +3610,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.03564267158508301</v>
+        <v>0.03611187934875489</v>
       </c>
       <c r="B11" t="n">
-        <v>0.01011568839605383</v>
+        <v>0.006390358987578264</v>
       </c>
       <c r="C11" t="n">
-        <v>0.01429157257080078</v>
+        <v>0.01468591690063476</v>
       </c>
       <c r="D11" t="n">
-        <v>0.00330125206206295</v>
+        <v>0.003865581265085115</v>
       </c>
       <c r="E11" t="n">
         <v>0.1</v>
@@ -3674,16 +3674,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.2577434539794922</v>
+        <v>0.2442879676818848</v>
       </c>
       <c r="B12" t="n">
-        <v>0.1174105678581004</v>
+        <v>0.05225107240309068</v>
       </c>
       <c r="C12" t="n">
-        <v>0.09125571250915528</v>
+        <v>0.0697669506072998</v>
       </c>
       <c r="D12" t="n">
-        <v>0.03702329886074172</v>
+        <v>0.01050518806000304</v>
       </c>
       <c r="E12" t="n">
         <v>0.1</v>
@@ -3738,16 +3738,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.2954594135284424</v>
+        <v>0.2490078449249268</v>
       </c>
       <c r="B13" t="n">
-        <v>0.0853920904155694</v>
+        <v>0.09173163283204763</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0812753677368164</v>
+        <v>0.09880356788635254</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0162705758403405</v>
+        <v>0.05209406888963723</v>
       </c>
       <c r="E13" t="n">
         <v>0.1</v>
@@ -3802,16 +3802,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.03082914352416992</v>
+        <v>0.05774526596069336</v>
       </c>
       <c r="B14" t="n">
-        <v>0.007482995683990156</v>
+        <v>0.01833922687644699</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0117030143737793</v>
+        <v>0.01787972450256348</v>
       </c>
       <c r="D14" t="n">
-        <v>0.003618938295026523</v>
+        <v>0.005948427936905906</v>
       </c>
       <c r="E14" t="n">
         <v>0.1</v>
@@ -3866,16 +3866,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.02884716987609863</v>
+        <v>0.03135914802551269</v>
       </c>
       <c r="B15" t="n">
-        <v>0.008155477731617827</v>
+        <v>0.01023979009572253</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01297111511230469</v>
+        <v>0.01621770858764648</v>
       </c>
       <c r="D15" t="n">
-        <v>0.005297621121244878</v>
+        <v>0.01138608460627852</v>
       </c>
       <c r="E15" t="n">
         <v>0.1</v>
@@ -3930,16 +3930,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.4642256736755371</v>
+        <v>0.4640603542327881</v>
       </c>
       <c r="B16" t="n">
-        <v>0.09037849088902351</v>
+        <v>0.09897946302220237</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02040300369262695</v>
+        <v>0.02615227699279785</v>
       </c>
       <c r="D16" t="n">
-        <v>0.002920514106881127</v>
+        <v>0.01276845692051451</v>
       </c>
       <c r="E16" t="n">
         <v>0.1</v>
@@ -3994,16 +3994,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.05175671577453613</v>
+        <v>0.06418385505676269</v>
       </c>
       <c r="B17" t="n">
-        <v>0.0139133010300651</v>
+        <v>0.01459266073012993</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01253194808959961</v>
+        <v>0.01866374015808105</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0031611546565935</v>
+        <v>0.007597888052509057</v>
       </c>
       <c r="E17" t="n">
         <v>0.1</v>
@@ -4058,16 +4058,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.02825832366943359</v>
+        <v>0.02044544219970703</v>
       </c>
       <c r="B18" t="n">
-        <v>0.01060775720004332</v>
+        <v>0.001888027612038162</v>
       </c>
       <c r="C18" t="n">
-        <v>0.009340858459472657</v>
+        <v>0.01052489280700684</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00217770907140333</v>
+        <v>0.003687051108693569</v>
       </c>
       <c r="E18" t="n">
         <v>1</v>
@@ -4122,16 +4122,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.01626763343811035</v>
+        <v>0.0284853458404541</v>
       </c>
       <c r="B19" t="n">
-        <v>0.002108367406661176</v>
+        <v>0.01211831618677749</v>
       </c>
       <c r="C19" t="n">
-        <v>0.006441354751586914</v>
+        <v>0.01418881416320801</v>
       </c>
       <c r="D19" t="n">
-        <v>0.001083672813479565</v>
+        <v>0.007568702405476075</v>
       </c>
       <c r="E19" t="n">
         <v>1</v>
@@ -4186,16 +4186,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.2465144634246826</v>
+        <v>0.22183518409729</v>
       </c>
       <c r="B20" t="n">
-        <v>0.0436381407575455</v>
+        <v>0.03029028271011538</v>
       </c>
       <c r="C20" t="n">
-        <v>0.04159693717956543</v>
+        <v>0.05809001922607422</v>
       </c>
       <c r="D20" t="n">
-        <v>0.01287206934294038</v>
+        <v>0.03101793643967419</v>
       </c>
       <c r="E20" t="n">
         <v>1</v>
@@ -4250,16 +4250,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.06553468704223633</v>
+        <v>0.09421029090881347</v>
       </c>
       <c r="B21" t="n">
-        <v>0.01162399149259167</v>
+        <v>0.02777023606747189</v>
       </c>
       <c r="C21" t="n">
-        <v>0.02103033065795899</v>
+        <v>0.01985611915588379</v>
       </c>
       <c r="D21" t="n">
-        <v>0.007103273634953586</v>
+        <v>0.01004824232835426</v>
       </c>
       <c r="E21" t="n">
         <v>1</v>
@@ -4314,16 +4314,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.03034467697143555</v>
+        <v>0.03060951232910156</v>
       </c>
       <c r="B22" t="n">
-        <v>0.006784815105893202</v>
+        <v>0.0127575071283235</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01210713386535645</v>
+        <v>0.01296095848083496</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00354947921664047</v>
+        <v>0.007321898714751551</v>
       </c>
       <c r="E22" t="n">
         <v>1</v>
@@ -4378,16 +4378,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.03664741516113281</v>
+        <v>0.02882447242736817</v>
       </c>
       <c r="B23" t="n">
-        <v>0.01096674566808661</v>
+        <v>0.009856475706214543</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01976957321166992</v>
+        <v>0.01766080856323242</v>
       </c>
       <c r="D23" t="n">
-        <v>0.009166889745663771</v>
+        <v>0.007584454330055439</v>
       </c>
       <c r="E23" t="n">
         <v>1</v>
@@ -4442,16 +4442,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.3755631923675537</v>
+        <v>0.397434139251709</v>
       </c>
       <c r="B24" t="n">
-        <v>0.04116122881721102</v>
+        <v>0.06081674922084607</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01886749267578125</v>
+        <v>0.01537408828735352</v>
       </c>
       <c r="D24" t="n">
-        <v>0.007174900004469256</v>
+        <v>0.003001545748835493</v>
       </c>
       <c r="E24" t="n">
         <v>1</v>
@@ -4506,16 +4506,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.05871124267578125</v>
+        <v>0.06005206108093262</v>
       </c>
       <c r="B25" t="n">
-        <v>0.02240989646451766</v>
+        <v>0.01518614972221106</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01051654815673828</v>
+        <v>0.01395978927612305</v>
       </c>
       <c r="D25" t="n">
-        <v>0.005084615629209348</v>
+        <v>0.002742434413133677</v>
       </c>
       <c r="E25" t="n">
         <v>1</v>
@@ -4570,16 +4570,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.02562646865844726</v>
+        <v>0.03358230590820312</v>
       </c>
       <c r="B26" t="n">
-        <v>0.01082635339673728</v>
+        <v>0.008696052943482351</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01165509223937988</v>
+        <v>0.01166830062866211</v>
       </c>
       <c r="D26" t="n">
-        <v>0.008846043617009547</v>
+        <v>0.003446972573953685</v>
       </c>
       <c r="E26" t="n">
         <v>1</v>
@@ -4634,16 +4634,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.02872762680053711</v>
+        <v>0.01556792259216309</v>
       </c>
       <c r="B27" t="n">
-        <v>0.0150380404606041</v>
+        <v>0.0003496810970880597</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01350569725036621</v>
+        <v>0.006830072402954102</v>
       </c>
       <c r="D27" t="n">
-        <v>0.006210444084839764</v>
+        <v>0.001186910719939126</v>
       </c>
       <c r="E27" t="n">
         <v>1</v>
@@ -4698,16 +4698,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.1251672267913818</v>
+        <v>0.1583560466766357</v>
       </c>
       <c r="B28" t="n">
-        <v>0.01365205920216024</v>
+        <v>0.04240422120888348</v>
       </c>
       <c r="C28" t="n">
-        <v>0.03494720458984375</v>
+        <v>0.04133086204528809</v>
       </c>
       <c r="D28" t="n">
-        <v>0.008276357393497219</v>
+        <v>0.01307921687695708</v>
       </c>
       <c r="E28" t="n">
         <v>1</v>
@@ -4762,16 +4762,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.1550321102142334</v>
+        <v>0.1313022613525391</v>
       </c>
       <c r="B29" t="n">
-        <v>0.01531629119159177</v>
+        <v>0.008832507937791353</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02855286598205566</v>
+        <v>0.02211565971374512</v>
       </c>
       <c r="D29" t="n">
-        <v>0.01075558572199369</v>
+        <v>0.004984625190591302</v>
       </c>
       <c r="E29" t="n">
         <v>1</v>
@@ -4826,16 +4826,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.03088803291320801</v>
+        <v>0.02868762016296387</v>
       </c>
       <c r="B30" t="n">
-        <v>0.008292146179141455</v>
+        <v>0.008223711868101101</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01307392120361328</v>
+        <v>0.01039190292358399</v>
       </c>
       <c r="D30" t="n">
-        <v>0.004889769220080741</v>
+        <v>0.0023337944282012</v>
       </c>
       <c r="E30" t="n">
         <v>1</v>
@@ -4890,16 +4890,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.02176012992858887</v>
+        <v>0.03283901214599609</v>
       </c>
       <c r="B31" t="n">
-        <v>0.006732213367712513</v>
+        <v>0.002766003551453363</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01022210121154785</v>
+        <v>0.02105116844177246</v>
       </c>
       <c r="D31" t="n">
-        <v>0.004084413897956878</v>
+        <v>0.008699010499406166</v>
       </c>
       <c r="E31" t="n">
         <v>1</v>
@@ -4954,16 +4954,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.3336957931518555</v>
+        <v>0.3036283969879151</v>
       </c>
       <c r="B32" t="n">
-        <v>0.02932009406373651</v>
+        <v>0.04878918087124831</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01147441864013672</v>
+        <v>0.01413993835449219</v>
       </c>
       <c r="D32" t="n">
-        <v>0.001377228114917613</v>
+        <v>0.002394476655889456</v>
       </c>
       <c r="E32" t="n">
         <v>1</v>
@@ -5018,16 +5018,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.05640401840209961</v>
+        <v>0.04728412628173828</v>
       </c>
       <c r="B33" t="n">
-        <v>0.02851019083334461</v>
+        <v>0.02679662129912054</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01262750625610352</v>
+        <v>0.00985870361328125</v>
       </c>
       <c r="D33" t="n">
-        <v>0.004951974445845827</v>
+        <v>0.003567519210333072</v>
       </c>
       <c r="E33" t="n">
         <v>1</v>
@@ -5082,16 +5082,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.02864608764648437</v>
+        <v>0.02730364799499512</v>
       </c>
       <c r="B34" t="n">
-        <v>0.007421080663716972</v>
+        <v>0.004171065416630073</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01236863136291504</v>
+        <v>0.01013660430908203</v>
       </c>
       <c r="D34" t="n">
-        <v>0.005758305404593382</v>
+        <v>0.002471579808120569</v>
       </c>
       <c r="E34" t="n">
         <v>10</v>
@@ -5146,16 +5146,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.02038545608520508</v>
+        <v>0.02273311614990235</v>
       </c>
       <c r="B35" t="n">
-        <v>0.00689638836653048</v>
+        <v>0.006951596343952159</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01080341339111328</v>
+        <v>0.009218692779541016</v>
       </c>
       <c r="D35" t="n">
-        <v>0.00490541433053682</v>
+        <v>0.002231611028657102</v>
       </c>
       <c r="E35" t="n">
         <v>10</v>
@@ -5210,16 +5210,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.1509881019592285</v>
+        <v>0.153862476348877</v>
       </c>
       <c r="B36" t="n">
-        <v>0.03955607719152569</v>
+        <v>0.03349968577935182</v>
       </c>
       <c r="C36" t="n">
-        <v>0.02520136833190918</v>
+        <v>0.02810688018798828</v>
       </c>
       <c r="D36" t="n">
-        <v>0.009402694936537366</v>
+        <v>0.01418739690425547</v>
       </c>
       <c r="E36" t="n">
         <v>10</v>
@@ -5274,16 +5274,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.09589581489562989</v>
+        <v>0.0880772590637207</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0243810649037597</v>
+        <v>0.02367471006463722</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0235870361328125</v>
+        <v>0.0205528736114502</v>
       </c>
       <c r="D37" t="n">
-        <v>0.01446288521821553</v>
+        <v>0.006005043427238599</v>
       </c>
       <c r="E37" t="n">
         <v>10</v>
@@ -5338,16 +5338,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.02305512428283691</v>
+        <v>0.03269028663635254</v>
       </c>
       <c r="B38" t="n">
-        <v>0.005470714916416858</v>
+        <v>0.009823720332878495</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01124477386474609</v>
+        <v>0.01118178367614746</v>
       </c>
       <c r="D38" t="n">
-        <v>0.003644183537327938</v>
+        <v>0.003094047089980215</v>
       </c>
       <c r="E38" t="n">
         <v>10</v>
@@ -5402,16 +5402,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.04356164932250976</v>
+        <v>0.02177448272705078</v>
       </c>
       <c r="B39" t="n">
-        <v>0.01705446637452877</v>
+        <v>0.006929336787644092</v>
       </c>
       <c r="C39" t="n">
-        <v>0.01612629890441895</v>
+        <v>0.009203338623046875</v>
       </c>
       <c r="D39" t="n">
-        <v>0.005058119108542377</v>
+        <v>0.001394371002770817</v>
       </c>
       <c r="E39" t="n">
         <v>10</v>
@@ -5466,16 +5466,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.2961014747619629</v>
+        <v>0.3004221439361572</v>
       </c>
       <c r="B40" t="n">
-        <v>0.08924507700627292</v>
+        <v>0.05740671815713614</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01243124008178711</v>
+        <v>0.01539392471313477</v>
       </c>
       <c r="D40" t="n">
-        <v>0.007538840056691077</v>
+        <v>0.01007466056376526</v>
       </c>
       <c r="E40" t="n">
         <v>10</v>
@@ -5530,16 +5530,16 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.05639901161193848</v>
+        <v>0.05132761001586914</v>
       </c>
       <c r="B41" t="n">
-        <v>0.01032116015981558</v>
+        <v>0.01536113799279811</v>
       </c>
       <c r="C41" t="n">
-        <v>0.01019191741943359</v>
+        <v>0.007125616073608398</v>
       </c>
       <c r="D41" t="n">
-        <v>0.002024002006129505</v>
+        <v>0.0008789423975075966</v>
       </c>
       <c r="E41" t="n">
         <v>10</v>
@@ -5594,16 +5594,16 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.03722858428955078</v>
+        <v>0.02694435119628906</v>
       </c>
       <c r="B42" t="n">
-        <v>0.01207142229333602</v>
+        <v>0.005256883536305507</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01416392326354981</v>
+        <v>0.008645248413085938</v>
       </c>
       <c r="D42" t="n">
-        <v>0.004560670371647072</v>
+        <v>0.002260205551540337</v>
       </c>
       <c r="E42" t="n">
         <v>10</v>
@@ -5658,16 +5658,16 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.01628227233886719</v>
+        <v>0.01636381149291992</v>
       </c>
       <c r="B43" t="n">
-        <v>0.00196848996794597</v>
+        <v>0.002941485817645424</v>
       </c>
       <c r="C43" t="n">
-        <v>0.006641483306884766</v>
+        <v>0.006408405303955078</v>
       </c>
       <c r="D43" t="n">
-        <v>0.001628257559623108</v>
+        <v>0.001386369325099937</v>
       </c>
       <c r="E43" t="n">
         <v>10</v>
@@ -5722,16 +5722,16 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.1298904895782471</v>
+        <v>0.1459310531616211</v>
       </c>
       <c r="B44" t="n">
-        <v>0.03840370215842268</v>
+        <v>0.01227026309241197</v>
       </c>
       <c r="C44" t="n">
-        <v>0.03327035903930664</v>
+        <v>0.02446298599243164</v>
       </c>
       <c r="D44" t="n">
-        <v>0.009019083751465238</v>
+        <v>0.007361729654015403</v>
       </c>
       <c r="E44" t="n">
         <v>10</v>
@@ -5786,16 +5786,16 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.05589971542358398</v>
+        <v>0.0630836009979248</v>
       </c>
       <c r="B45" t="n">
-        <v>0.009334686913607473</v>
+        <v>0.0406155228051751</v>
       </c>
       <c r="C45" t="n">
-        <v>0.01518650054931641</v>
+        <v>0.01733870506286621</v>
       </c>
       <c r="D45" t="n">
-        <v>0.005653452093341975</v>
+        <v>0.007429278703851054</v>
       </c>
       <c r="E45" t="n">
         <v>10</v>
@@ -5850,16 +5850,16 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.0292294979095459</v>
+        <v>0.0146395206451416</v>
       </c>
       <c r="B46" t="n">
-        <v>0.005383190406778263</v>
+        <v>0.00388214742663139</v>
       </c>
       <c r="C46" t="n">
-        <v>0.009924793243408203</v>
+        <v>0.005051422119140625</v>
       </c>
       <c r="D46" t="n">
-        <v>0.002703488496260394</v>
+        <v>0.0003886951015565357</v>
       </c>
       <c r="E46" t="n">
         <v>10</v>
@@ -5914,16 +5914,16 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.01713428497314453</v>
+        <v>0.01829347610473633</v>
       </c>
       <c r="B47" t="n">
-        <v>0.007970305825031889</v>
+        <v>0.006193796496555096</v>
       </c>
       <c r="C47" t="n">
-        <v>0.01068720817565918</v>
+        <v>0.008722448348999023</v>
       </c>
       <c r="D47" t="n">
-        <v>0.008974173672235413</v>
+        <v>0.001603354819879154</v>
       </c>
       <c r="E47" t="n">
         <v>10</v>
@@ -5978,16 +5978,16 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.1810742378234863</v>
+        <v>0.2060820579528809</v>
       </c>
       <c r="B48" t="n">
-        <v>0.07744617658613476</v>
+        <v>0.09457747906151558</v>
       </c>
       <c r="C48" t="n">
-        <v>0.005713844299316406</v>
+        <v>0.006368017196655274</v>
       </c>
       <c r="D48" t="n">
-        <v>0.0003304972962993957</v>
+        <v>0.001625919462306117</v>
       </c>
       <c r="E48" t="n">
         <v>10</v>
@@ -6042,16 +6042,16 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.04582509994506836</v>
+        <v>0.05044760704040527</v>
       </c>
       <c r="B49" t="n">
-        <v>0.023982966272589</v>
+        <v>0.02072734313949632</v>
       </c>
       <c r="C49" t="n">
-        <v>0.008390140533447266</v>
+        <v>0.01492114067077637</v>
       </c>
       <c r="D49" t="n">
-        <v>0.003314234844512141</v>
+        <v>0.005904136423098981</v>
       </c>
       <c r="E49" t="n">
         <v>10</v>
@@ -6217,16 +6217,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.3041504859924317</v>
+        <v>0.2958269119262695</v>
       </c>
       <c r="B2" t="n">
-        <v>0.02684356271213288</v>
+        <v>0.02020571414588377</v>
       </c>
       <c r="C2" t="n">
-        <v>0.01824502944946289</v>
+        <v>0.01534638404846191</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00311039180303603</v>
+        <v>0.001417765903406797</v>
       </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="n">
@@ -6273,16 +6273,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>0.3159913063049317</v>
+        <v>0.3502821445465088</v>
       </c>
       <c r="B3" t="n">
-        <v>0.008502293544980312</v>
+        <v>0.02126039270363875</v>
       </c>
       <c r="C3" t="n">
-        <v>0.01681103706359863</v>
+        <v>0.0178257942199707</v>
       </c>
       <c r="D3" t="n">
-        <v>0.003353779861768459</v>
+        <v>0.003042460410500076</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
@@ -6329,16 +6329,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.6013609409332276</v>
+        <v>0.5856868267059326</v>
       </c>
       <c r="B4" t="n">
-        <v>0.04151242350011761</v>
+        <v>0.03600511707838328</v>
       </c>
       <c r="C4" t="n">
-        <v>0.02651925086975098</v>
+        <v>0.02620849609375</v>
       </c>
       <c r="D4" t="n">
-        <v>0.002967485624780861</v>
+        <v>0.003077262157780125</v>
       </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
@@ -6385,16 +6385,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>0.6353859424591064</v>
+        <v>0.6674427509307861</v>
       </c>
       <c r="B5" t="n">
-        <v>0.02784309444329952</v>
+        <v>0.04484098429618533</v>
       </c>
       <c r="C5" t="n">
-        <v>0.02824854850769043</v>
+        <v>0.02695760726928711</v>
       </c>
       <c r="D5" t="n">
-        <v>0.005235236567576628</v>
+        <v>0.00397905566466614</v>
       </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
@@ -6441,16 +6441,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.2982461929321289</v>
+        <v>0.2877766609191895</v>
       </c>
       <c r="B6" t="n">
-        <v>0.02386303541933906</v>
+        <v>0.02190216639929089</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01640219688415527</v>
+        <v>0.01479077339172363</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001476353878261887</v>
+        <v>0.0006283776643204065</v>
       </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
@@ -6497,16 +6497,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>0.3321562767028808</v>
+        <v>0.3237441062927246</v>
       </c>
       <c r="B7" t="n">
-        <v>0.03002600910346339</v>
+        <v>0.006594419961913649</v>
       </c>
       <c r="C7" t="n">
-        <v>0.01755051612854004</v>
+        <v>0.01618680953979492</v>
       </c>
       <c r="D7" t="n">
-        <v>0.002729926589689211</v>
+        <v>0.001227118165077544</v>
       </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
@@ -6553,16 +6553,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.568495512008667</v>
+        <v>0.6182753086090088</v>
       </c>
       <c r="B8" t="n">
-        <v>0.03528830253998393</v>
+        <v>0.06145001628721251</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02538962364196777</v>
+        <v>0.02522835731506348</v>
       </c>
       <c r="D8" t="n">
-        <v>0.003408777767616983</v>
+        <v>0.003198100488963286</v>
       </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="n">
@@ -6609,16 +6609,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>0.6422585010528564</v>
+        <v>0.7049998283386231</v>
       </c>
       <c r="B9" t="n">
-        <v>0.08092967453851896</v>
+        <v>0.06637976293096892</v>
       </c>
       <c r="C9" t="n">
-        <v>0.02653837203979492</v>
+        <v>0.02687458992004394</v>
       </c>
       <c r="D9" t="n">
-        <v>0.00236050104331201</v>
+        <v>0.003154776953937709</v>
       </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="n">
@@ -6665,16 +6665,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2927299499511719</v>
+        <v>0.2788980007171631</v>
       </c>
       <c r="B10" t="n">
-        <v>0.03186376028896629</v>
+        <v>0.01807754245835672</v>
       </c>
       <c r="C10" t="n">
-        <v>0.01687984466552734</v>
+        <v>0.01447267532348633</v>
       </c>
       <c r="D10" t="n">
-        <v>0.002843801393455058</v>
+        <v>0.001133251739934557</v>
       </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="n">
@@ -6721,16 +6721,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>0.3483455657958984</v>
+        <v>0.3437389373779297</v>
       </c>
       <c r="B11" t="n">
-        <v>0.04667947726046948</v>
+        <v>0.03399640359024586</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0209136962890625</v>
+        <v>0.02101969718933105</v>
       </c>
       <c r="D11" t="n">
-        <v>0.006915333607795914</v>
+        <v>0.003673691412132166</v>
       </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
@@ -6777,16 +6777,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.5743406295776368</v>
+        <v>0.5844845771789551</v>
       </c>
       <c r="B12" t="n">
-        <v>0.04510222661339556</v>
+        <v>0.03287056178141251</v>
       </c>
       <c r="C12" t="n">
-        <v>0.02414383888244629</v>
+        <v>0.02419872283935547</v>
       </c>
       <c r="D12" t="n">
-        <v>0.001078669455923698</v>
+        <v>0.001738326281636231</v>
       </c>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
@@ -6833,16 +6833,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>0.6618286609649658</v>
+        <v>0.6863741874694824</v>
       </c>
       <c r="B13" t="n">
-        <v>0.04263695678026605</v>
+        <v>0.04716338535549034</v>
       </c>
       <c r="C13" t="n">
-        <v>0.02734708786010742</v>
+        <v>0.02698898315429688</v>
       </c>
       <c r="D13" t="n">
-        <v>0.002998317698289188</v>
+        <v>0.002217570538710776</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
@@ -6889,16 +6889,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.2881369113922119</v>
+        <v>0.2749049186706543</v>
       </c>
       <c r="B14" t="n">
-        <v>0.03529091216723228</v>
+        <v>0.007838795826256312</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0153684139251709</v>
+        <v>0.01396327018737793</v>
       </c>
       <c r="D14" t="n">
-        <v>0.001495070114353302</v>
+        <v>0.000469306740556033</v>
       </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="n">
@@ -6945,16 +6945,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.3654116630554199</v>
+        <v>0.3560141563415528</v>
       </c>
       <c r="B15" t="n">
-        <v>0.03590513550709444</v>
+        <v>0.04497512082018089</v>
       </c>
       <c r="C15" t="n">
-        <v>0.03606739044189453</v>
+        <v>0.01892557144165039</v>
       </c>
       <c r="D15" t="n">
-        <v>0.01281769059636913</v>
+        <v>0.002562903480496987</v>
       </c>
       <c r="E15" t="inlineStr"/>
       <c r="F15" t="n">
@@ -7001,16 +7001,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.6560186386108399</v>
+        <v>0.6236851215362549</v>
       </c>
       <c r="B16" t="n">
-        <v>0.04081842867977352</v>
+        <v>0.04039302239606974</v>
       </c>
       <c r="C16" t="n">
-        <v>0.02687735557556152</v>
+        <v>0.03202238082885742</v>
       </c>
       <c r="D16" t="n">
-        <v>0.004194709628792067</v>
+        <v>0.007472519481137458</v>
       </c>
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="n">
@@ -7057,16 +7057,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0.7490833282470704</v>
+        <v>0.7013503551483155</v>
       </c>
       <c r="B17" t="n">
-        <v>0.06797479502579927</v>
+        <v>0.1135067482346414</v>
       </c>
       <c r="C17" t="n">
-        <v>0.02671570777893066</v>
+        <v>0.02609000205993652</v>
       </c>
       <c r="D17" t="n">
-        <v>0.003563874458795069</v>
+        <v>0.001342591314332887</v>
       </c>
       <c r="E17" t="inlineStr"/>
       <c r="F17" t="n">
@@ -7113,16 +7113,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.2876410007476807</v>
+        <v>0.3022891521453858</v>
       </c>
       <c r="B18" t="n">
-        <v>0.01587345835070982</v>
+        <v>0.01612549194661375</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01472830772399902</v>
+        <v>0.01808433532714844</v>
       </c>
       <c r="D18" t="n">
-        <v>0.001158625232350626</v>
+        <v>0.007696111580886944</v>
       </c>
       <c r="E18" t="n">
         <v>10</v>
@@ -7171,16 +7171,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0.334312105178833</v>
+        <v>0.3514134883880615</v>
       </c>
       <c r="B19" t="n">
-        <v>0.02550444749026195</v>
+        <v>0.02890476408485871</v>
       </c>
       <c r="C19" t="n">
-        <v>0.01749267578125</v>
+        <v>0.01704916954040527</v>
       </c>
       <c r="D19" t="n">
-        <v>0.001314208638246143</v>
+        <v>0.002755660789545396</v>
       </c>
       <c r="E19" t="n">
         <v>10</v>
@@ -7229,16 +7229,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.5603192329406739</v>
+        <v>0.6451800346374512</v>
       </c>
       <c r="B20" t="n">
-        <v>0.03823776563149739</v>
+        <v>0.1199514283472944</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02473893165588379</v>
+        <v>0.02932538986206055</v>
       </c>
       <c r="D20" t="n">
-        <v>0.00309266403044303</v>
+        <v>0.004940183141075128</v>
       </c>
       <c r="E20" t="n">
         <v>10</v>
@@ -7287,16 +7287,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0.646356201171875</v>
+        <v>0.6984891891479492</v>
       </c>
       <c r="B21" t="n">
-        <v>0.05075980034323822</v>
+        <v>0.0446288289003325</v>
       </c>
       <c r="C21" t="n">
-        <v>0.02737584114074707</v>
+        <v>0.02711343765258789</v>
       </c>
       <c r="D21" t="n">
-        <v>0.002990302720408264</v>
+        <v>0.00439056909996712</v>
       </c>
       <c r="E21" t="n">
         <v>10</v>
@@ -7345,16 +7345,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.2747166633605957</v>
+        <v>0.3563690662384033</v>
       </c>
       <c r="B22" t="n">
-        <v>0.01309259421857756</v>
+        <v>0.08466114928875086</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01493315696716309</v>
+        <v>0.02125988006591797</v>
       </c>
       <c r="D22" t="n">
-        <v>0.002599059212222494</v>
+        <v>0.009782963571982979</v>
       </c>
       <c r="E22" t="n">
         <v>10</v>
@@ -7403,16 +7403,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0.3506791114807129</v>
+        <v>0.3682597637176513</v>
       </c>
       <c r="B23" t="n">
-        <v>0.03109261002636898</v>
+        <v>0.05798573702928077</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01747426986694336</v>
+        <v>0.01629142761230469</v>
       </c>
       <c r="D23" t="n">
-        <v>0.004893532875183819</v>
+        <v>0.001056394551585524</v>
       </c>
       <c r="E23" t="n">
         <v>10</v>
@@ -7461,16 +7461,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.5998172283172607</v>
+        <v>0.5708157539367675</v>
       </c>
       <c r="B24" t="n">
-        <v>0.03898136884566596</v>
+        <v>0.04605736265528113</v>
       </c>
       <c r="C24" t="n">
-        <v>0.02387576103210449</v>
+        <v>0.0251929759979248</v>
       </c>
       <c r="D24" t="n">
-        <v>0.001436262534141047</v>
+        <v>0.001983737599407815</v>
       </c>
       <c r="E24" t="n">
         <v>10</v>
@@ -7519,16 +7519,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0.769077730178833</v>
+        <v>0.7246158123016357</v>
       </c>
       <c r="B25" t="n">
-        <v>0.04086404849520216</v>
+        <v>0.04991899576261333</v>
       </c>
       <c r="C25" t="n">
-        <v>0.02660908699035645</v>
+        <v>0.02919383049011231</v>
       </c>
       <c r="D25" t="n">
-        <v>0.002691766654339782</v>
+        <v>0.004652231131338487</v>
       </c>
       <c r="E25" t="n">
         <v>10</v>
@@ -7577,16 +7577,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.3131368637084961</v>
+        <v>0.287867021560669</v>
       </c>
       <c r="B26" t="n">
-        <v>0.05072372322914516</v>
+        <v>0.01821332850925886</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01457624435424805</v>
+        <v>0.01838669776916504</v>
       </c>
       <c r="D26" t="n">
-        <v>0.001142133371152278</v>
+        <v>0.005692337996214036</v>
       </c>
       <c r="E26" t="n">
         <v>10</v>
@@ -7635,16 +7635,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0.3604159355163574</v>
+        <v>0.3280497550964355</v>
       </c>
       <c r="B27" t="n">
-        <v>0.06534996875156514</v>
+        <v>0.01781281884422218</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01740989685058594</v>
+        <v>0.01711664199829101</v>
       </c>
       <c r="D27" t="n">
-        <v>0.003024183588432019</v>
+        <v>0.002521238043111182</v>
       </c>
       <c r="E27" t="n">
         <v>10</v>
@@ -7693,16 +7693,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.5760008335113526</v>
+        <v>0.5604515552520752</v>
       </c>
       <c r="B28" t="n">
-        <v>0.05209653379657909</v>
+        <v>0.02832619119414559</v>
       </c>
       <c r="C28" t="n">
-        <v>0.02462220191955566</v>
+        <v>0.02470536231994629</v>
       </c>
       <c r="D28" t="n">
-        <v>0.001449213568581359</v>
+        <v>0.002310359421869608</v>
       </c>
       <c r="E28" t="n">
         <v>10</v>
@@ -7751,16 +7751,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.6472743034362793</v>
+        <v>0.6569996356964112</v>
       </c>
       <c r="B29" t="n">
-        <v>0.0388544908732209</v>
+        <v>0.03118805112651883</v>
       </c>
       <c r="C29" t="n">
-        <v>0.02831196784973145</v>
+        <v>0.02887067794799805</v>
       </c>
       <c r="D29" t="n">
-        <v>0.003767600729002051</v>
+        <v>0.004130126056264732</v>
       </c>
       <c r="E29" t="n">
         <v>10</v>
@@ -7809,16 +7809,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.2832871913909912</v>
+        <v>0.2691638946533203</v>
       </c>
       <c r="B30" t="n">
-        <v>0.02900935601683801</v>
+        <v>0.01210777905576254</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01744508743286133</v>
+        <v>0.01472735404968262</v>
       </c>
       <c r="D30" t="n">
-        <v>0.006616095482735598</v>
+        <v>0.0008872478007062918</v>
       </c>
       <c r="E30" t="n">
         <v>10</v>
@@ -7867,16 +7867,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.3293128490447998</v>
+        <v>0.3274716377258301</v>
       </c>
       <c r="B31" t="n">
-        <v>0.01456741079944184</v>
+        <v>0.03043294869188587</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01599359512329102</v>
+        <v>0.01675982475280762</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0005481075232026161</v>
+        <v>0.002651367862305722</v>
       </c>
       <c r="E31" t="n">
         <v>10</v>
@@ -7925,16 +7925,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.578593397140503</v>
+        <v>0.5874533653259277</v>
       </c>
       <c r="B32" t="n">
-        <v>0.06937198872100918</v>
+        <v>0.05354679266268635</v>
       </c>
       <c r="C32" t="n">
-        <v>0.02544589042663574</v>
+        <v>0.02605633735656738</v>
       </c>
       <c r="D32" t="n">
-        <v>0.003637952682827057</v>
+        <v>0.002821055891165201</v>
       </c>
       <c r="E32" t="n">
         <v>10</v>
@@ -7983,16 +7983,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0.6203779220581055</v>
+        <v>0.6415965557098389</v>
       </c>
       <c r="B33" t="n">
-        <v>0.02101219125241495</v>
+        <v>0.02541301616662889</v>
       </c>
       <c r="C33" t="n">
-        <v>0.02702302932739258</v>
+        <v>0.02875065803527832</v>
       </c>
       <c r="D33" t="n">
-        <v>0.002909662712600075</v>
+        <v>0.00236258959628778</v>
       </c>
       <c r="E33" t="n">
         <v>10</v>
@@ -8041,16 +8041,16 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0.28537278175354</v>
+        <v>0.2804548740386963</v>
       </c>
       <c r="B34" t="n">
-        <v>0.01663880335244062</v>
+        <v>0.01556560627568549</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01450858116149902</v>
+        <v>0.01540555953979492</v>
       </c>
       <c r="D34" t="n">
-        <v>0.0006938072675900861</v>
+        <v>0.0007351684357527132</v>
       </c>
       <c r="E34" t="n">
         <v>20</v>
@@ -8099,16 +8099,16 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0.3396347999572754</v>
+        <v>0.3324438095092773</v>
       </c>
       <c r="B35" t="n">
-        <v>0.03914665501448995</v>
+        <v>0.01874619218112513</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01800541877746582</v>
+        <v>0.01684150695800781</v>
       </c>
       <c r="D35" t="n">
-        <v>0.003705842313928405</v>
+        <v>0.001278941622585787</v>
       </c>
       <c r="E35" t="n">
         <v>20</v>
@@ -8157,16 +8157,16 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0.5518327236175538</v>
+        <v>0.6002527236938476</v>
       </c>
       <c r="B36" t="n">
-        <v>0.03322488312990739</v>
+        <v>0.05898742552664924</v>
       </c>
       <c r="C36" t="n">
-        <v>0.02389273643493652</v>
+        <v>0.02640681266784668</v>
       </c>
       <c r="D36" t="n">
-        <v>0.0008290886651857893</v>
+        <v>0.002451057289479097</v>
       </c>
       <c r="E36" t="n">
         <v>20</v>
@@ -8215,16 +8215,16 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0.6393847465515137</v>
+        <v>0.6324922561645507</v>
       </c>
       <c r="B37" t="n">
-        <v>0.0396174015603798</v>
+        <v>0.02050919946038994</v>
       </c>
       <c r="C37" t="n">
-        <v>0.02461519241333008</v>
+        <v>0.02671055793762207</v>
       </c>
       <c r="D37" t="n">
-        <v>0.0009226496836916326</v>
+        <v>0.001027786898676842</v>
       </c>
       <c r="E37" t="n">
         <v>20</v>
@@ -8273,16 +8273,16 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0.3029354095458984</v>
+        <v>0.3257069110870361</v>
       </c>
       <c r="B38" t="n">
-        <v>0.03067955704200262</v>
+        <v>0.04385948662639649</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01475424766540527</v>
+        <v>0.01990466117858887</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0005763067268824456</v>
+        <v>0.006394648357044831</v>
       </c>
       <c r="E38" t="n">
         <v>20</v>
@@ -8331,16 +8331,16 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0.3164714336395263</v>
+        <v>0.3686078071594238</v>
       </c>
       <c r="B39" t="n">
-        <v>0.01473573748398266</v>
+        <v>0.05953060597682242</v>
       </c>
       <c r="C39" t="n">
-        <v>0.01644024848937988</v>
+        <v>0.0163276195526123</v>
       </c>
       <c r="D39" t="n">
-        <v>0.001075519012234604</v>
+        <v>0.001662825591849968</v>
       </c>
       <c r="E39" t="n">
         <v>20</v>
@@ -8389,16 +8389,16 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0.6010930061340332</v>
+        <v>0.5717700481414795</v>
       </c>
       <c r="B40" t="n">
-        <v>0.05805725567880207</v>
+        <v>0.0356560154442155</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0233522891998291</v>
+        <v>0.0293571949005127</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0006114547899161266</v>
+        <v>0.01061967662638765</v>
       </c>
       <c r="E40" t="n">
         <v>20</v>
@@ -8447,16 +8447,16 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0.6514202117919922</v>
+        <v>0.690358304977417</v>
       </c>
       <c r="B41" t="n">
-        <v>0.03998738326611338</v>
+        <v>0.08339117210491546</v>
       </c>
       <c r="C41" t="n">
-        <v>0.02867279052734375</v>
+        <v>0.02681803703308105</v>
       </c>
       <c r="D41" t="n">
-        <v>0.004815856378526361</v>
+        <v>0.003713943306975416</v>
       </c>
       <c r="E41" t="n">
         <v>20</v>
@@ -8505,16 +8505,16 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0.2796150207519531</v>
+        <v>0.304823637008667</v>
       </c>
       <c r="B42" t="n">
-        <v>0.01319149708828831</v>
+        <v>0.02836965718188969</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01496405601501465</v>
+        <v>0.01693840026855469</v>
       </c>
       <c r="D42" t="n">
-        <v>0.001168446207287175</v>
+        <v>0.005108294700719777</v>
       </c>
       <c r="E42" t="n">
         <v>20</v>
@@ -8563,16 +8563,16 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0.3590517044067383</v>
+        <v>0.3336862087249756</v>
       </c>
       <c r="B43" t="n">
-        <v>0.03279738657375141</v>
+        <v>0.02200361481055106</v>
       </c>
       <c r="C43" t="n">
-        <v>0.01952323913574219</v>
+        <v>0.01563920974731445</v>
       </c>
       <c r="D43" t="n">
-        <v>0.005237236142374713</v>
+        <v>0.0009362319001716717</v>
       </c>
       <c r="E43" t="n">
         <v>20</v>
@@ -8621,16 +8621,16 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0.5831630229949951</v>
+        <v>0.5755544185638428</v>
       </c>
       <c r="B44" t="n">
-        <v>0.04671928470988205</v>
+        <v>0.0443550482342174</v>
       </c>
       <c r="C44" t="n">
-        <v>0.02399682998657227</v>
+        <v>0.02697410583496094</v>
       </c>
       <c r="D44" t="n">
-        <v>0.001833549330004531</v>
+        <v>0.003966816654992152</v>
       </c>
       <c r="E44" t="n">
         <v>20</v>
@@ -8679,16 +8679,16 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0.6650797367095947</v>
+        <v>0.626926040649414</v>
       </c>
       <c r="B45" t="n">
-        <v>0.02827654758236395</v>
+        <v>0.04047129124248659</v>
       </c>
       <c r="C45" t="n">
-        <v>0.02799720764160156</v>
+        <v>0.02718033790588379</v>
       </c>
       <c r="D45" t="n">
-        <v>0.003265277327390262</v>
+        <v>0.001777954255689506</v>
       </c>
       <c r="E45" t="n">
         <v>20</v>
@@ -8737,16 +8737,16 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0.3188194274902344</v>
+        <v>0.2831298351287842</v>
       </c>
       <c r="B46" t="n">
-        <v>0.03094376164102479</v>
+        <v>0.02828865582797882</v>
       </c>
       <c r="C46" t="n">
-        <v>0.01556110382080078</v>
+        <v>0.01588234901428223</v>
       </c>
       <c r="D46" t="n">
-        <v>0.001121074460300354</v>
+        <v>0.0020306371003239</v>
       </c>
       <c r="E46" t="n">
         <v>20</v>
@@ -8795,16 +8795,16 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0.324685001373291</v>
+        <v>0.3485227108001709</v>
       </c>
       <c r="B47" t="n">
-        <v>0.01232352939687857</v>
+        <v>0.04064616377377994</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0160771369934082</v>
+        <v>0.01660237312316894</v>
       </c>
       <c r="D47" t="n">
-        <v>0.001477546277202616</v>
+        <v>0.001223797950498109</v>
       </c>
       <c r="E47" t="n">
         <v>20</v>
@@ -8853,16 +8853,16 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0.5206279754638672</v>
+        <v>0.4989845752716064</v>
       </c>
       <c r="B48" t="n">
-        <v>0.01268083147659357</v>
+        <v>0.02693338505912797</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0189633846282959</v>
+        <v>0.01748833656311035</v>
       </c>
       <c r="D48" t="n">
-        <v>0.003463450571725237</v>
+        <v>0.002813381754828632</v>
       </c>
       <c r="E48" t="n">
         <v>20</v>
@@ -8911,16 +8911,16 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0.5105763435363769</v>
+        <v>0.5116800308227539</v>
       </c>
       <c r="B49" t="n">
-        <v>0.04139541943980554</v>
+        <v>0.04799554453151965</v>
       </c>
       <c r="C49" t="n">
-        <v>0.01301479339599609</v>
+        <v>0.01286311149597168</v>
       </c>
       <c r="D49" t="n">
-        <v>0.000993357841354518</v>
+        <v>0.00102989599848605</v>
       </c>
       <c r="E49" t="n">
         <v>20</v>
@@ -9080,16 +9080,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.2401586532592773</v>
+        <v>0.2278040885925293</v>
       </c>
       <c r="B2" t="n">
-        <v>0.009087172331574678</v>
+        <v>0.004937397149645039</v>
       </c>
       <c r="C2" t="n">
-        <v>0.004668092727661133</v>
+        <v>0.004578638076782227</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0004211451480275677</v>
+        <v>0.0001575493639197839</v>
       </c>
       <c r="E2" t="n">
         <v>0.01</v>
@@ -9138,16 +9138,16 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.898581981658936</v>
+        <v>1.987168264389038</v>
       </c>
       <c r="B3" t="n">
-        <v>0.2060345288182105</v>
+        <v>0.09842691202987125</v>
       </c>
       <c r="C3" t="n">
-        <v>0.005904245376586914</v>
+        <v>0.005258035659790039</v>
       </c>
       <c r="D3" t="n">
-        <v>0.001144679230378271</v>
+        <v>0.0004831363031656717</v>
       </c>
       <c r="E3" t="n">
         <v>0.01</v>
@@ -9196,16 +9196,16 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>0.2567145824432373</v>
+        <v>0.2784756183624267</v>
       </c>
       <c r="B4" t="n">
-        <v>0.01802189773903016</v>
+        <v>0.02039781053593129</v>
       </c>
       <c r="C4" t="n">
-        <v>0.004496574401855469</v>
+        <v>0.005597209930419922</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0008907735848484715</v>
+        <v>0.001291368720924959</v>
       </c>
       <c r="E4" t="n">
         <v>0.01</v>
@@ -9254,16 +9254,16 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1.654277658462525</v>
+        <v>1.681682920455933</v>
       </c>
       <c r="B5" t="n">
-        <v>0.1479305672738842</v>
+        <v>0.08424852745831422</v>
       </c>
       <c r="C5" t="n">
-        <v>0.005382490158081055</v>
+        <v>0.005423164367675782</v>
       </c>
       <c r="D5" t="n">
-        <v>0.0007579423511410323</v>
+        <v>0.0006843923084479614</v>
       </c>
       <c r="E5" t="n">
         <v>0.01</v>
@@ -9312,16 +9312,16 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>0.4479108333587646</v>
+        <v>0.4653010845184326</v>
       </c>
       <c r="B6" t="n">
-        <v>0.007294543976189943</v>
+        <v>0.0224161382333016</v>
       </c>
       <c r="C6" t="n">
-        <v>0.004062366485595703</v>
+        <v>0.004253005981445313</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0002456434106486777</v>
+        <v>0.0001271667218133905</v>
       </c>
       <c r="E6" t="n">
         <v>0.01</v>
@@ -9370,16 +9370,16 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>4.243521308898925</v>
+        <v>4.465656709671021</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6117736078663776</v>
+        <v>0.1926863506532195</v>
       </c>
       <c r="C7" t="n">
-        <v>0.005854940414428711</v>
+        <v>0.005522680282592773</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0008317479120643862</v>
+        <v>0.0004108336198799247</v>
       </c>
       <c r="E7" t="n">
         <v>0.01</v>
@@ -9428,16 +9428,16 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>0.4484874248504639</v>
+        <v>0.4901026248931885</v>
       </c>
       <c r="B8" t="n">
-        <v>0.02038803978618396</v>
+        <v>0.03026845051877209</v>
       </c>
       <c r="C8" t="n">
-        <v>0.004520988464355469</v>
+        <v>0.00429534912109375</v>
       </c>
       <c r="D8" t="n">
-        <v>0.000559154256872762</v>
+        <v>0.0002243160792857192</v>
       </c>
       <c r="E8" t="n">
         <v>0.01</v>
@@ -9486,16 +9486,16 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2.892759990692139</v>
+        <v>2.944373035430908</v>
       </c>
       <c r="B9" t="n">
-        <v>0.1761674541072087</v>
+        <v>0.1932622129744223</v>
       </c>
       <c r="C9" t="n">
-        <v>0.00531930923461914</v>
+        <v>0.00528569221496582</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0003911865331495267</v>
+        <v>0.0006108575712708246</v>
       </c>
       <c r="E9" t="n">
         <v>0.01</v>
@@ -9544,16 +9544,16 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>0.2709400653839111</v>
+        <v>0.252858829498291</v>
       </c>
       <c r="B10" t="n">
-        <v>0.02391768388550839</v>
+        <v>0.009495280454285427</v>
       </c>
       <c r="C10" t="n">
-        <v>0.004219818115234375</v>
+        <v>0.004961204528808594</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0002452424265992402</v>
+        <v>0.001232275566776823</v>
       </c>
       <c r="E10" t="n">
         <v>0.01</v>
@@ -9602,16 +9602,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2.094063329696655</v>
+        <v>2.388978719711304</v>
       </c>
       <c r="B11" t="n">
-        <v>0.4567856599838101</v>
+        <v>0.3617414104597856</v>
       </c>
       <c r="C11" t="n">
-        <v>0.005532073974609375</v>
+        <v>0.00650181770324707</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0004811052849768247</v>
+        <v>0.002929714995617786</v>
       </c>
       <c r="E11" t="n">
         <v>0.01</v>
@@ -9660,16 +9660,16 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.2814150333404541</v>
+        <v>0.2655713081359863</v>
       </c>
       <c r="B12" t="n">
-        <v>0.01175634344811262</v>
+        <v>0.02354636212093307</v>
       </c>
       <c r="C12" t="n">
-        <v>0.005054140090942382</v>
+        <v>0.00431985855102539</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0007657662802076743</v>
+        <v>0.00062559345850583</v>
       </c>
       <c r="E12" t="n">
         <v>0.01</v>
@@ -9718,16 +9718,16 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1.806627655029297</v>
+        <v>1.819629621505737</v>
       </c>
       <c r="B13" t="n">
-        <v>0.09183279303018771</v>
+        <v>0.1103349619014754</v>
       </c>
       <c r="C13" t="n">
-        <v>0.005228042602539062</v>
+        <v>0.005365276336669922</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0002571757899667009</v>
+        <v>0.000514200939577703</v>
       </c>
       <c r="E13" t="n">
         <v>0.01</v>
@@ -9776,16 +9776,16 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>0.4736497402191162</v>
+        <v>0.4733738899230957</v>
       </c>
       <c r="B14" t="n">
-        <v>0.02464794017089383</v>
+        <v>0.01860322467144144</v>
       </c>
       <c r="C14" t="n">
-        <v>0.004346418380737305</v>
+        <v>0.005267715454101563</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0004849299660609243</v>
+        <v>0.001269978367290952</v>
       </c>
       <c r="E14" t="n">
         <v>0.01</v>
@@ -9834,16 +9834,16 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5.045019054412842</v>
+        <v>5.402458667755127</v>
       </c>
       <c r="B15" t="n">
-        <v>0.7404273992688811</v>
+        <v>0.8769298417192123</v>
       </c>
       <c r="C15" t="n">
-        <v>0.006202936172485352</v>
+        <v>0.005261135101318359</v>
       </c>
       <c r="D15" t="n">
-        <v>0.00133909710586234</v>
+        <v>0.0001575443848354106</v>
       </c>
       <c r="E15" t="n">
         <v>0.01</v>
@@ -9892,16 +9892,16 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0.4999983787536621</v>
+        <v>0.5134970188140869</v>
       </c>
       <c r="B16" t="n">
-        <v>0.05152516055296706</v>
+        <v>0.05968311048387675</v>
       </c>
       <c r="C16" t="n">
-        <v>0.00557413101196289</v>
+        <v>0.005191850662231445</v>
       </c>
       <c r="D16" t="n">
-        <v>0.001593796003582809</v>
+        <v>0.0003356089675552479</v>
       </c>
       <c r="E16" t="n">
         <v>0.01</v>
@@ -9950,16 +9950,16 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>3.21928596496582</v>
+        <v>3.103811979293823</v>
       </c>
       <c r="B17" t="n">
-        <v>0.08875789952259636</v>
+        <v>0.1063751775390017</v>
       </c>
       <c r="C17" t="n">
-        <v>0.005117082595825195</v>
+        <v>0.005261850357055664</v>
       </c>
       <c r="D17" t="n">
-        <v>0.0003275178713934078</v>
+        <v>0.0003987100180872502</v>
       </c>
       <c r="E17" t="n">
         <v>0.01</v>
@@ -10008,16 +10008,16 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0.2477166175842285</v>
+        <v>0.230049991607666</v>
       </c>
       <c r="B18" t="n">
-        <v>0.03014696982804575</v>
+        <v>0.02613584885887539</v>
       </c>
       <c r="C18" t="n">
-        <v>0.005932855606079102</v>
+        <v>0.00392756462097168</v>
       </c>
       <c r="D18" t="n">
-        <v>0.002261874581507816</v>
+        <v>0.0001811207179338508</v>
       </c>
       <c r="E18" t="n">
         <v>0.1</v>
@@ -10066,16 +10066,16 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1.747190618515015</v>
+        <v>1.724667119979858</v>
       </c>
       <c r="B19" t="n">
-        <v>0.1922428214602743</v>
+        <v>0.3378083392950943</v>
       </c>
       <c r="C19" t="n">
-        <v>0.006471824645996094</v>
+        <v>0.005274724960327148</v>
       </c>
       <c r="D19" t="n">
-        <v>0.002133950840396957</v>
+        <v>0.0005025952635163662</v>
       </c>
       <c r="E19" t="n">
         <v>0.1</v>
@@ -10124,16 +10124,16 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0.2167123794555664</v>
+        <v>0.2211357116699219</v>
       </c>
       <c r="B20" t="n">
-        <v>0.01250422359739094</v>
+        <v>0.01344810757426153</v>
       </c>
       <c r="C20" t="n">
-        <v>0.005112552642822265</v>
+        <v>0.004402637481689453</v>
       </c>
       <c r="D20" t="n">
-        <v>0.001987452382312324</v>
+        <v>0.0006160547117754282</v>
       </c>
       <c r="E20" t="n">
         <v>0.1</v>
@@ -10182,16 +10182,16 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>1.238561820983887</v>
+        <v>1.231485748291016</v>
       </c>
       <c r="B21" t="n">
-        <v>0.07387230303769379</v>
+        <v>0.09874725791095139</v>
       </c>
       <c r="C21" t="n">
-        <v>0.004969406127929688</v>
+        <v>0.005667877197265625</v>
       </c>
       <c r="D21" t="n">
-        <v>0.0005009295517927941</v>
+        <v>0.001143253412355752</v>
       </c>
       <c r="E21" t="n">
         <v>0.1</v>
@@ -10240,16 +10240,16 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0.3924705982208252</v>
+        <v>0.3892970561981201</v>
       </c>
       <c r="B22" t="n">
-        <v>0.03042320613480646</v>
+        <v>0.009432842614677318</v>
       </c>
       <c r="C22" t="n">
-        <v>0.004624700546264649</v>
+        <v>0.004415035247802734</v>
       </c>
       <c r="D22" t="n">
-        <v>0.001032468055876938</v>
+        <v>0.0003722193727973537</v>
       </c>
       <c r="E22" t="n">
         <v>0.1</v>
@@ -10298,16 +10298,16 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2.362762308120728</v>
+        <v>2.488258266448975</v>
       </c>
       <c r="B23" t="n">
-        <v>0.2505844605466726</v>
+        <v>0.4477520247147929</v>
       </c>
       <c r="C23" t="n">
-        <v>0.005105018615722656</v>
+        <v>0.005164194107055664</v>
       </c>
       <c r="D23" t="n">
-        <v>0.000399264155356063</v>
+        <v>0.0002609240294169344</v>
       </c>
       <c r="E23" t="n">
         <v>0.1</v>
@@ -10356,16 +10356,16 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0.3902744293212891</v>
+        <v>0.3950511455535889</v>
       </c>
       <c r="B24" t="n">
-        <v>0.01572385880190723</v>
+        <v>0.02671847547416273</v>
       </c>
       <c r="C24" t="n">
-        <v>0.004595708847045898</v>
+        <v>0.004832172393798828</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0005758549245751034</v>
+        <v>0.0007626578973756498</v>
       </c>
       <c r="E24" t="n">
         <v>0.1</v>
@@ -10414,16 +10414,16 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2.169717359542847</v>
+        <v>2.170387935638428</v>
       </c>
       <c r="B25" t="n">
-        <v>0.08337673752030446</v>
+        <v>0.09721657611981852</v>
       </c>
       <c r="C25" t="n">
-        <v>0.005681180953979492</v>
+        <v>0.005866098403930664</v>
       </c>
       <c r="D25" t="n">
-        <v>0.001183116895259458</v>
+        <v>0.00111794140120275</v>
       </c>
       <c r="E25" t="n">
         <v>0.1</v>
@@ -10472,16 +10472,16 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0.2140758037567139</v>
+        <v>0.2231451511383057</v>
       </c>
       <c r="B26" t="n">
-        <v>0.009819848793288099</v>
+        <v>0.01028733361061927</v>
       </c>
       <c r="C26" t="n">
-        <v>0.004513788223266602</v>
+        <v>0.004168510437011719</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0007001414851403017</v>
+        <v>0.0003740351519636346</v>
       </c>
       <c r="E26" t="n">
         <v>0.1</v>
@@ -10530,16 +10530,16 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1.821027135848999</v>
+        <v>1.557092094421387</v>
       </c>
       <c r="B27" t="n">
-        <v>0.3813412305592101</v>
+        <v>0.2359614548846886</v>
       </c>
       <c r="C27" t="n">
-        <v>0.004994726181030274</v>
+        <v>0.005808973312377929</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0002251075247721263</v>
+        <v>0.000738866071431923</v>
       </c>
       <c r="E27" t="n">
         <v>0.1</v>
@@ -10588,16 +10588,16 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0.2089676856994629</v>
+        <v>0.2205078601837158</v>
       </c>
       <c r="B28" t="n">
-        <v>0.007993444235284936</v>
+        <v>0.01140045818780994</v>
       </c>
       <c r="C28" t="n">
-        <v>0.00424036979675293</v>
+        <v>0.00412149429321289</v>
       </c>
       <c r="D28" t="n">
-        <v>0.00062359866966993</v>
+        <v>0.0003178151818046214</v>
       </c>
       <c r="E28" t="n">
         <v>0.1</v>
@@ -10646,16 +10646,16 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1.250311136245728</v>
+        <v>1.29622917175293</v>
       </c>
       <c r="B29" t="n">
-        <v>0.05486910667510827</v>
+        <v>0.08028174712228001</v>
       </c>
       <c r="C29" t="n">
-        <v>0.004732418060302735</v>
+        <v>0.005247783660888672</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0003103897999037927</v>
+        <v>0.0006801178785638975</v>
       </c>
       <c r="E29" t="n">
         <v>0.1</v>
@@ -10704,16 +10704,16 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0.4078182220458985</v>
+        <v>0.4144733905792236</v>
       </c>
       <c r="B30" t="n">
-        <v>0.02651471252917241</v>
+        <v>0.03373572888209279</v>
       </c>
       <c r="C30" t="n">
-        <v>0.004967164993286133</v>
+        <v>0.004173660278320312</v>
       </c>
       <c r="D30" t="n">
-        <v>0.001214255401810783</v>
+        <v>0.0001657109360441852</v>
       </c>
       <c r="E30" t="n">
         <v>0.1</v>
@@ -10762,16 +10762,16 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2.328103542327881</v>
+        <v>2.40603461265564</v>
       </c>
       <c r="B31" t="n">
-        <v>0.2183064480313682</v>
+        <v>0.2444550790598887</v>
       </c>
       <c r="C31" t="n">
-        <v>0.003396463394165039</v>
+        <v>0.003897476196289063</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0007654456668196479</v>
+        <v>0.0009295453264045432</v>
       </c>
       <c r="E31" t="n">
         <v>0.1</v>
@@ -10820,16 +10820,16 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.4025423049926758</v>
+        <v>0.3908119678497314</v>
       </c>
       <c r="B32" t="n">
-        <v>0.01726131812502799</v>
+        <v>0.01841857006458894</v>
       </c>
       <c r="C32" t="n">
-        <v>0.004160118103027344</v>
+        <v>0.005478668212890625</v>
       </c>
       <c r="D32" t="n">
-        <v>0.0004039746393410334</v>
+        <v>0.002541943546131004</v>
       </c>
       <c r="E32" t="n">
         <v>0.1</v>
@@ -10878,16 +10878,16 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1.756406402587891</v>
+        <v>1.821315717697144</v>
       </c>
       <c r="B33" t="n">
-        <v>0.08980579306050827</v>
+        <v>0.04892649464718569</v>
       </c>
       <c r="C33" t="n">
-        <v>0.003134632110595703</v>
+        <v>0.002837944030761719</v>
       </c>
       <c r="D33" t="n">
-        <v>0.0002346404461938297</v>
+        <v>0.0004009881670294328</v>
       </c>
       <c r="E33" t="n">
         <v>0.1</v>

</xml_diff>